<commit_message>
[SMAL] Edit template QMM007
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM007会社一律金額の登録.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM007会社一律金額の登録.xlsx
@@ -647,13 +647,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>90488</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>4763</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>149544</xdr:rowOff>
@@ -44308,468 +44308,471 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:J40"/>
+  <dimension ref="C2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="1" customWidth="1"/>
-    <col min="6" max="10" width="12" style="1" customWidth="1"/>
-    <col min="11" max="11" width="1.140625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.5703125" style="1"/>
+    <col min="1" max="1" width="10.5703125" style="1"/>
+    <col min="2" max="2" width="1.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="1" customWidth="1"/>
+    <col min="7" max="11" width="12" style="1" customWidth="1"/>
+    <col min="12" max="12" width="1.140625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="3:11">
+      <c r="C2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="E2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="G2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="16"/>
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
-      <c r="J2" s="17"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="17"/>
     </row>
-    <row r="3" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B3" s="19"/>
-      <c r="C3" s="21"/>
+    <row r="3" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C3" s="19"/>
       <c r="D3" s="21"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="21"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B4" s="9"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="5"/>
+    <row r="4" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C4" s="9"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="11"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B5" s="10"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="7"/>
+    <row r="5" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C5" s="10"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B6" s="9"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="5"/>
+    <row r="6" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C6" s="9"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B7" s="10"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="7"/>
+    <row r="7" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C7" s="10"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B8" s="9"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="5"/>
+    <row r="8" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C8" s="9"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B9" s="10"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="7"/>
+    <row r="9" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C9" s="10"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B10" s="9"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="5"/>
+    <row r="10" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C10" s="9"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B11" s="10"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="7"/>
+    <row r="11" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C11" s="10"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B12" s="9"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="5"/>
+    <row r="12" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C12" s="9"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B13" s="10"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="7"/>
+    <row r="13" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C13" s="10"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B14" s="9"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="5"/>
+    <row r="14" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C14" s="9"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B15" s="10"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="7"/>
+    <row r="15" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C15" s="10"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="14"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B16" s="9"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="5"/>
+    <row r="16" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C16" s="9"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B17" s="10"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="7"/>
+    <row r="17" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C17" s="10"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="14"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B18" s="9"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="5"/>
+    <row r="18" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C18" s="9"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B19" s="10"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="7"/>
+    <row r="19" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C19" s="10"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="14"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B20" s="9"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="5"/>
+    <row r="20" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C20" s="9"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B21" s="10"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="7"/>
+    <row r="21" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C21" s="10"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="14"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B22" s="9"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="5"/>
+    <row r="22" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C22" s="9"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B23" s="10"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="7"/>
+    <row r="23" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C23" s="10"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B24" s="9"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="5"/>
+    <row r="24" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C24" s="9"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="13"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B25" s="10"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="7"/>
+    <row r="25" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C25" s="10"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="14"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B26" s="9"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="5"/>
+    <row r="26" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C26" s="9"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="13"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B27" s="10"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="7"/>
+    <row r="27" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C27" s="10"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="14"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B28" s="9"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="5"/>
+    <row r="28" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C28" s="9"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="13"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B29" s="10"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="7"/>
+    <row r="29" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C29" s="10"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="14"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B30" s="9"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="5"/>
+    <row r="30" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C30" s="9"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="13"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B31" s="10"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="7"/>
+    <row r="31" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C31" s="10"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="14"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
     </row>
-    <row r="32" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B32" s="9"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="5"/>
+    <row r="32" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C32" s="9"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="13"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
     </row>
-    <row r="33" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B33" s="10"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="7"/>
+    <row r="33" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C33" s="10"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="14"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B34" s="9"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="5"/>
+    <row r="34" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C34" s="9"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="13"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
     </row>
-    <row r="35" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B35" s="10"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="7"/>
+    <row r="35" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C35" s="10"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="14"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B36" s="9"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="5"/>
+    <row r="36" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C36" s="9"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="13"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
     </row>
-    <row r="37" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B37" s="10"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="7"/>
+    <row r="37" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C37" s="10"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="14"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B38" s="9"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="5"/>
+    <row r="38" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C38" s="9"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="13"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
     </row>
-    <row r="39" spans="2:10" ht="13.15" customHeight="1">
-      <c r="B39" s="10"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="7"/>
+    <row r="39" spans="3:11" ht="13.15" customHeight="1">
+      <c r="C39" s="10"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="14"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="2:10" ht="13.15" customHeight="1"/>
+    <row r="40" spans="3:11" ht="13.15" customHeight="1"/>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="G2:K2"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.2" right="0.2" top="0.75" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[SMAL] QMM007 Fix bug 1439
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM007会社一律金額の登録.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM007会社一律金額の登録.xlsx
@@ -648,15 +648,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>90488</xdr:colOff>
+      <xdr:colOff>90489</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>149544</xdr:rowOff>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -665,8 +665,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="90488" y="304801"/>
-          <a:ext cx="8235315" cy="5178743"/>
+          <a:off x="842964" y="152401"/>
+          <a:ext cx="8443912" cy="6143624"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6390,7 +6390,8 @@
             <v>FT1200 ﾓﾃﾞﾙ 6300-40N</v>
           </cell>
           <cell r="F5" t="str">
-            <v>PentiumⅡ-300､ﾒﾓﾘ:64MB､HDD:4GB､16倍速CD-ROM､100BASE-TX､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､WindowsNT Server 4.0(10ｸﾗｲｱﾝﾄﾗｲｾﾝｽ付き)</v>
+            <v>PentiumⅡ-300､ﾒﾓﾘ:64MB､HDD:4GB､16倍速CD-ROM､100BASE-TX､
+ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､WindowsNT Server 4.0(10ｸﾗｲｱﾝﾄﾗｲｾﾝｽ付き)</v>
           </cell>
           <cell r="G5">
             <v>1</v>
@@ -6425,8 +6426,8 @@
           <cell r="Z5" t="str">
             <v>AC</v>
           </cell>
-          <cell r="AA5" t="str">
-            <v/>
+          <cell r="AA5">
+            <v>0</v>
           </cell>
         </row>
         <row r="6">
@@ -6475,8 +6476,8 @@
           <cell r="Z6" t="str">
             <v>AC</v>
           </cell>
-          <cell r="AA6" t="str">
-            <v/>
+          <cell r="AA6">
+            <v>0</v>
           </cell>
         </row>
         <row r="7">
@@ -6487,10 +6488,12 @@
             <v>M6346-1</v>
           </cell>
           <cell r="E7" t="str">
-            <v>15ｲﾝﾁ高解像度ｶﾗｰﾃﾞｨｽﾌﾟﾚｲ</v>
+            <v>15ｲﾝﾁ高解像度
+ｶﾗｰﾃﾞｨｽﾌﾟﾚｲ</v>
           </cell>
           <cell r="F7" t="str">
-            <v>FT//ex､FT1200､FT2200､FT2400､LS660､LS550､LS100､AL､EL､SX(M3423-Cﾓﾃﾞﾙ､M3423C-A3C0/B181)､FX､GX用｡</v>
+            <v>FT//ex､FT1200､FT2200､FT2400､LS660､LS550､LS100､AL､EL､
+SX(M3423-Cﾓﾃﾞﾙ､M3423C-A3C0/B181)､FX､GX用｡</v>
           </cell>
           <cell r="G7">
             <v>1</v>
@@ -6526,7 +6529,8 @@
             <v>AC</v>
           </cell>
           <cell r="AA7" t="str">
-            <v>本体同時購入割引実施中</v>
+            <v>本体同時購入
+割引実施中</v>
           </cell>
         </row>
         <row r="8">
@@ -6575,8 +6579,8 @@
           <cell r="Z8" t="str">
             <v>AC</v>
           </cell>
-          <cell r="AA8" t="str">
-            <v/>
+          <cell r="AA8">
+            <v>0</v>
           </cell>
         </row>
         <row r="9">
@@ -6590,7 +6594,9 @@
             <v>増設SCSI制御装置</v>
           </cell>
           <cell r="F9" t="str">
-            <v>FT1200､FT2200に内蔵高速ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(M6700-13)､または内蔵ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(M6700-15)を増設する場合に必要｡ISA｡但し､FT2200は内蔵ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(M6700-15）を未ｻﾎﾟｰﾄ｡</v>
+            <v>FT1200､FT2200に内蔵高速ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(M6700-13)､または
+内蔵ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(M6700-15)を増設する場合に必要｡ISA｡
+但し､FT2200は内蔵ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(M6700-15）を未ｻﾎﾟｰﾄ｡</v>
           </cell>
           <cell r="G9">
             <v>1</v>
@@ -6625,8 +6631,8 @@
           <cell r="Z9" t="str">
             <v>AC</v>
           </cell>
-          <cell r="AA9" t="str">
-            <v/>
+          <cell r="AA9">
+            <v>0</v>
           </cell>
         </row>
         <row r="10">
@@ -6637,7 +6643,8 @@
             <v>M6700-15</v>
           </cell>
           <cell r="E10" t="str">
-            <v>内蔵ｽﾄﾘ-ﾐﾝｸﾞﾃ-ﾌﾟ装置(DDS-3)</v>
+            <v>内蔵ｽﾄﾘ-ﾐﾝｸﾞﾃ-ﾌﾟ装置
+(DDS-3)</v>
           </cell>
           <cell r="F10" t="str">
             <v>FT1200､FT2400用｡12GB｡</v>
@@ -6675,8 +6682,8 @@
           <cell r="Z10" t="str">
             <v>AC</v>
           </cell>
-          <cell r="AA10" t="str">
-            <v/>
+          <cell r="AA10">
+            <v>0</v>
           </cell>
         </row>
         <row r="11">
@@ -6690,7 +6697,9 @@
             <v>LS550 ﾓﾃﾞﾙ 5200M-21CXA</v>
           </cell>
           <cell r="F11" t="str">
-            <v>MMX Pentium-200､ﾒﾓﾘ:32MB､HDD:2.1GB､最大16倍速CD-ROM､100BASE-TX､ｻｳﾝﾄﾞ機能､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､ﾃﾞｽｸﾄｯﾌﾟ管理ｿﾌﾄｳｪｱ､Windows95</v>
+            <v>MMX Pentium-200､ﾒﾓﾘ:32MB､HDD:2.1GB､最大16倍速CD-ROM､
+100BASE-TX､ｻｳﾝﾄﾞ機能､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､ﾃﾞｽｸﾄｯﾌﾟ管理ｿﾌﾄｳｪｱ､
+Windows95</v>
           </cell>
           <cell r="G11">
             <v>6</v>
@@ -6725,8 +6734,8 @@
           <cell r="Z11" t="str">
             <v>AC</v>
           </cell>
-          <cell r="AA11" t="str">
-            <v/>
+          <cell r="AA11">
+            <v>0</v>
           </cell>
         </row>
         <row r="12">
@@ -6740,7 +6749,8 @@
             <v>16MB増設SDRAMﾒﾓﾘｷｯﾄ</v>
           </cell>
           <cell r="F12" t="str">
-            <v>LS660(M3561)､LS550(M3552､M3555､M3558)用｡16MB SDRAM DIMM×1個｡</v>
+            <v>LS660(M3561)､LS550(M3552､M3555､M3558)用｡
+16MB SDRAM DIMM×1個｡</v>
           </cell>
           <cell r="G12">
             <v>6</v>
@@ -6775,8 +6785,8 @@
           <cell r="Z12" t="str">
             <v>AC</v>
           </cell>
-          <cell r="AA12" t="str">
-            <v/>
+          <cell r="AA12">
+            <v>0</v>
           </cell>
         </row>
         <row r="13">
@@ -6787,10 +6797,12 @@
             <v>M6346-1</v>
           </cell>
           <cell r="E13" t="str">
-            <v>15ｲﾝﾁ高解像度ｶﾗｰﾃﾞｨｽﾌﾟﾚｲ</v>
+            <v>15ｲﾝﾁ高解像度
+ｶﾗｰﾃﾞｨｽﾌﾟﾚｲ</v>
           </cell>
           <cell r="F13" t="str">
-            <v>FT//ex､FT1200､FT2200､FT2400､LS660､LS550､LS100､AL､EL､SX(M3423-Cﾓﾃﾞﾙ､M3423C-A3C0/B181)､FX､GX用｡</v>
+            <v>FT//ex､FT1200､FT2200､FT2400､LS660､LS550､LS100､AL､EL､
+SX(M3423-Cﾓﾃﾞﾙ､M3423C-A3C0/B181)､FX､GX用｡</v>
           </cell>
           <cell r="G13">
             <v>6</v>
@@ -6826,7 +6838,8 @@
             <v>AC</v>
           </cell>
           <cell r="AA13" t="str">
-            <v>本体同時購入割引実施中</v>
+            <v>本体同時購入
+割引実施中</v>
           </cell>
         </row>
         <row r="14">
@@ -6840,7 +6853,8 @@
             <v>日本語ﾗｲﾝﾌﾟﾘﾝﾀ</v>
           </cell>
           <cell r="F14" t="str">
-            <v>FT//s､FT//e､FT//ex（M3517､M3518､M3519､M3520､M3521)､LS660､LS550､XEN-PC､XEN-LSⅡ用｡430行/分(高速ﾓｰﾄﾞ)｡</v>
+            <v>FT//s､FT//e､FT//ex（M3517､M3518､M3519､M3520､M3521)､LS660､
+LS550､XEN-PC､XEN-LSⅡ用｡430行/分(高速ﾓｰﾄﾞ)｡</v>
           </cell>
           <cell r="G14">
             <v>1</v>
@@ -6875,8 +6889,8 @@
           <cell r="Z14" t="str">
             <v>MC</v>
           </cell>
-          <cell r="AA14" t="str">
-            <v/>
+          <cell r="AA14">
+            <v>0</v>
           </cell>
         </row>
         <row r="15">
@@ -6890,7 +6904,8 @@
             <v>ﾌﾟﾘﾝﾀｹｰﾌﾞﾙ</v>
           </cell>
           <cell r="F15" t="str">
-            <v>日本語ﾌﾟﾘﾝﾀ(M6261-1､M6265-1､M6267-1)､OA日本語ﾌﾟﾘﾝﾀ(M6268-1)､ﾍﾟｰｼﾞﾌﾟﾘﾝﾀ(M6257-1)､日本語ﾗｲﾝﾌﾟﾘﾝﾀ(M6611-1)用｡3m｡</v>
+            <v>日本語ﾌﾟﾘﾝﾀ(M6261-1､M6265-1､M6267-1)､OA日本語ﾌﾟﾘﾝﾀ(M6268-1)､
+ﾍﾟｰｼﾞﾌﾟﾘﾝﾀ(M6257-1)､日本語ﾗｲﾝﾌﾟﾘﾝﾀ(M6611-1)用｡3m｡</v>
           </cell>
           <cell r="G15">
             <v>1</v>
@@ -6925,8 +6940,8 @@
           <cell r="Z15" t="str">
             <v>MC</v>
           </cell>
-          <cell r="AA15" t="str">
-            <v/>
+          <cell r="AA15">
+            <v>0</v>
           </cell>
         </row>
         <row r="16">
@@ -6951,11 +6966,11 @@
           <cell r="L16">
             <v>60000</v>
           </cell>
-          <cell r="N16" t="str">
-            <v/>
-          </cell>
-          <cell r="P16" t="str">
-            <v/>
+          <cell r="N16">
+            <v>0</v>
+          </cell>
+          <cell r="P16">
+            <v>0</v>
           </cell>
           <cell r="R16">
             <v>421200</v>
@@ -6969,16 +6984,16 @@
           <cell r="X16">
             <v>0</v>
           </cell>
-          <cell r="Z16" t="str">
-            <v/>
-          </cell>
-          <cell r="AA16" t="str">
-            <v/>
+          <cell r="Z16">
+            <v>0</v>
+          </cell>
+          <cell r="AA16">
+            <v>0</v>
           </cell>
         </row>
         <row r="17">
-          <cell r="D17" t="str">
-            <v/>
+          <cell r="D17">
+            <v>0</v>
           </cell>
           <cell r="E17" t="str">
             <v>ﾌﾟﾘﾝﾀｹｰﾌﾞﾙ</v>
@@ -6998,11 +7013,11 @@
           <cell r="L17">
             <v>0</v>
           </cell>
-          <cell r="N17" t="str">
-            <v/>
-          </cell>
-          <cell r="P17" t="str">
-            <v/>
+          <cell r="N17">
+            <v>0</v>
+          </cell>
+          <cell r="P17">
+            <v>0</v>
           </cell>
           <cell r="R17">
             <v>1300</v>
@@ -7016,22 +7031,22 @@
           <cell r="X17">
             <v>0</v>
           </cell>
-          <cell r="Z17" t="str">
-            <v/>
-          </cell>
-          <cell r="AA17" t="str">
-            <v/>
+          <cell r="Z17">
+            <v>0</v>
+          </cell>
+          <cell r="AA17">
+            <v>0</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="D18" t="str">
-            <v/>
+          <cell r="D18">
+            <v>0</v>
           </cell>
           <cell r="E18" t="str">
             <v>ハンディターミナル  ＢＨＴ－６０００（１ＭＢ）</v>
           </cell>
-          <cell r="F18" t="str">
-            <v/>
+          <cell r="F18">
+            <v>0</v>
           </cell>
           <cell r="G18">
             <v>6</v>
@@ -7045,11 +7060,11 @@
           <cell r="L18">
             <v>0</v>
           </cell>
-          <cell r="N18" t="str">
-            <v/>
-          </cell>
-          <cell r="P18" t="str">
-            <v/>
+          <cell r="N18">
+            <v>0</v>
+          </cell>
+          <cell r="P18">
+            <v>0</v>
           </cell>
           <cell r="R18">
             <v>138600</v>
@@ -7063,22 +7078,22 @@
           <cell r="X18">
             <v>0</v>
           </cell>
-          <cell r="Z18" t="str">
-            <v/>
-          </cell>
-          <cell r="AA18" t="str">
-            <v/>
+          <cell r="Z18">
+            <v>0</v>
+          </cell>
+          <cell r="AA18">
+            <v>0</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="D19" t="str">
-            <v/>
+          <cell r="D19">
+            <v>0</v>
           </cell>
           <cell r="E19" t="str">
             <v>光通信ユニット</v>
           </cell>
-          <cell r="F19" t="str">
-            <v/>
+          <cell r="F19">
+            <v>0</v>
           </cell>
           <cell r="G19">
             <v>2</v>
@@ -7092,11 +7107,11 @@
           <cell r="L19">
             <v>0</v>
           </cell>
-          <cell r="N19" t="str">
-            <v/>
-          </cell>
-          <cell r="P19" t="str">
-            <v/>
+          <cell r="N19">
+            <v>0</v>
+          </cell>
+          <cell r="P19">
+            <v>0</v>
           </cell>
           <cell r="R19">
             <v>46000</v>
@@ -7110,22 +7125,22 @@
           <cell r="X19">
             <v>0</v>
           </cell>
-          <cell r="Z19" t="str">
-            <v/>
-          </cell>
-          <cell r="AA19" t="str">
-            <v/>
+          <cell r="Z19">
+            <v>0</v>
+          </cell>
+          <cell r="AA19">
+            <v>0</v>
           </cell>
         </row>
         <row r="20">
-          <cell r="D20" t="str">
-            <v/>
+          <cell r="D20">
+            <v>0</v>
           </cell>
           <cell r="E20" t="str">
             <v>ＮｉＭＨバッテリーパック</v>
           </cell>
-          <cell r="F20" t="str">
-            <v/>
+          <cell r="F20">
+            <v>0</v>
           </cell>
           <cell r="G20">
             <v>6</v>
@@ -7139,11 +7154,11 @@
           <cell r="L20">
             <v>0</v>
           </cell>
-          <cell r="N20" t="str">
-            <v/>
-          </cell>
-          <cell r="P20" t="str">
-            <v/>
+          <cell r="N20">
+            <v>0</v>
+          </cell>
+          <cell r="P20">
+            <v>0</v>
           </cell>
           <cell r="R20">
             <v>6000</v>
@@ -7157,22 +7172,22 @@
           <cell r="X20">
             <v>0</v>
           </cell>
-          <cell r="Z20" t="str">
-            <v/>
-          </cell>
-          <cell r="AA20" t="str">
-            <v/>
+          <cell r="Z20">
+            <v>0</v>
+          </cell>
+          <cell r="AA20">
+            <v>0</v>
           </cell>
         </row>
         <row r="21">
-          <cell r="D21" t="str">
-            <v/>
+          <cell r="D21">
+            <v>0</v>
           </cell>
           <cell r="E21" t="str">
             <v>ＲＳ２３２Ｃケーブル</v>
           </cell>
-          <cell r="F21" t="str">
-            <v/>
+          <cell r="F21">
+            <v>0</v>
           </cell>
           <cell r="G21">
             <v>2</v>
@@ -7186,11 +7201,11 @@
           <cell r="L21">
             <v>0</v>
           </cell>
-          <cell r="N21" t="str">
-            <v/>
-          </cell>
-          <cell r="P21" t="str">
-            <v/>
+          <cell r="N21">
+            <v>0</v>
+          </cell>
+          <cell r="P21">
+            <v>0</v>
           </cell>
           <cell r="R21">
             <v>9000</v>
@@ -7204,22 +7219,22 @@
           <cell r="X21">
             <v>0</v>
           </cell>
-          <cell r="Z21" t="str">
-            <v/>
-          </cell>
-          <cell r="AA21" t="str">
-            <v/>
+          <cell r="Z21">
+            <v>0</v>
+          </cell>
+          <cell r="AA21">
+            <v>0</v>
           </cell>
         </row>
         <row r="22">
-          <cell r="D22" t="str">
-            <v/>
+          <cell r="D22">
+            <v>0</v>
           </cell>
           <cell r="E22" t="str">
             <v>ＣＵ転送ユーティリティ</v>
           </cell>
-          <cell r="F22" t="str">
-            <v/>
+          <cell r="F22">
+            <v>0</v>
           </cell>
           <cell r="G22">
             <v>1</v>
@@ -7233,11 +7248,11 @@
           <cell r="L22">
             <v>0</v>
           </cell>
-          <cell r="N22" t="str">
-            <v/>
-          </cell>
-          <cell r="P22" t="str">
-            <v/>
+          <cell r="N22">
+            <v>0</v>
+          </cell>
+          <cell r="P22">
+            <v>0</v>
           </cell>
           <cell r="R22">
             <v>35000</v>
@@ -7251,22 +7266,22 @@
           <cell r="X22">
             <v>0</v>
           </cell>
-          <cell r="Z22" t="str">
-            <v/>
-          </cell>
-          <cell r="AA22" t="str">
-            <v/>
+          <cell r="Z22">
+            <v>0</v>
+          </cell>
+          <cell r="AA22">
+            <v>0</v>
           </cell>
         </row>
         <row r="23">
-          <cell r="D23" t="str">
-            <v/>
+          <cell r="D23">
+            <v>0</v>
           </cell>
           <cell r="E23" t="str">
             <v>ＢＨＴ－ＢＡＳＩＣ３，１</v>
           </cell>
-          <cell r="F23" t="str">
-            <v/>
+          <cell r="F23">
+            <v>0</v>
           </cell>
           <cell r="G23">
             <v>1</v>
@@ -7280,11 +7295,11 @@
           <cell r="L23">
             <v>0</v>
           </cell>
-          <cell r="N23" t="str">
-            <v/>
-          </cell>
-          <cell r="P23" t="str">
-            <v/>
+          <cell r="N23">
+            <v>0</v>
+          </cell>
+          <cell r="P23">
+            <v>0</v>
           </cell>
           <cell r="R23">
             <v>32000</v>
@@ -7298,22 +7313,22 @@
           <cell r="X23">
             <v>0</v>
           </cell>
-          <cell r="Z23" t="str">
-            <v/>
-          </cell>
-          <cell r="AA23" t="str">
-            <v/>
+          <cell r="Z23">
+            <v>0</v>
+          </cell>
+          <cell r="AA23">
+            <v>0</v>
           </cell>
         </row>
         <row r="24">
-          <cell r="D24" t="str">
-            <v/>
+          <cell r="D24">
+            <v>0</v>
           </cell>
           <cell r="E24" t="str">
             <v>ＨＵＢ</v>
           </cell>
-          <cell r="F24" t="str">
-            <v/>
+          <cell r="F24">
+            <v>0</v>
           </cell>
           <cell r="G24">
             <v>3</v>
@@ -7327,11 +7342,11 @@
           <cell r="L24">
             <v>0</v>
           </cell>
-          <cell r="N24" t="str">
-            <v/>
-          </cell>
-          <cell r="P24" t="str">
-            <v/>
+          <cell r="N24">
+            <v>0</v>
+          </cell>
+          <cell r="P24">
+            <v>0</v>
           </cell>
           <cell r="R24">
             <v>11000</v>
@@ -7345,22 +7360,22 @@
           <cell r="X24">
             <v>0</v>
           </cell>
-          <cell r="Z24" t="str">
-            <v/>
-          </cell>
-          <cell r="AA24" t="str">
-            <v/>
+          <cell r="Z24">
+            <v>0</v>
+          </cell>
+          <cell r="AA24">
+            <v>0</v>
           </cell>
         </row>
         <row r="25">
-          <cell r="D25" t="str">
-            <v/>
+          <cell r="D25">
+            <v>0</v>
           </cell>
           <cell r="E25" t="str">
             <v>10BASE-Tｹｰﾌﾞﾙ</v>
           </cell>
-          <cell r="F25" t="str">
-            <v/>
+          <cell r="F25">
+            <v>0</v>
           </cell>
           <cell r="G25">
             <v>10</v>
@@ -7374,11 +7389,11 @@
           <cell r="L25">
             <v>0</v>
           </cell>
-          <cell r="N25" t="str">
-            <v/>
-          </cell>
-          <cell r="P25" t="str">
-            <v/>
+          <cell r="N25">
+            <v>0</v>
+          </cell>
+          <cell r="P25">
+            <v>0</v>
           </cell>
           <cell r="R25">
             <v>3200</v>
@@ -7392,22 +7407,22 @@
           <cell r="X25">
             <v>0</v>
           </cell>
-          <cell r="Z25" t="str">
-            <v/>
-          </cell>
-          <cell r="AA25" t="str">
-            <v/>
+          <cell r="Z25">
+            <v>0</v>
+          </cell>
+          <cell r="AA25">
+            <v>0</v>
           </cell>
         </row>
         <row r="26">
-          <cell r="D26" t="str">
-            <v/>
+          <cell r="D26">
+            <v>0</v>
           </cell>
           <cell r="E26" t="str">
             <v>Microsoft Office97</v>
           </cell>
-          <cell r="F26" t="str">
-            <v/>
+          <cell r="F26">
+            <v>0</v>
           </cell>
           <cell r="G26">
             <v>1</v>
@@ -7421,11 +7436,11 @@
           <cell r="L26">
             <v>0</v>
           </cell>
-          <cell r="N26" t="str">
-            <v/>
-          </cell>
-          <cell r="P26" t="str">
-            <v/>
+          <cell r="N26">
+            <v>0</v>
+          </cell>
+          <cell r="P26">
+            <v>0</v>
           </cell>
           <cell r="R26">
             <v>55000</v>
@@ -7439,22 +7454,22 @@
           <cell r="X26">
             <v>0</v>
           </cell>
-          <cell r="Z26" t="str">
-            <v/>
-          </cell>
-          <cell r="AA26" t="str">
-            <v/>
+          <cell r="Z26">
+            <v>0</v>
+          </cell>
+          <cell r="AA26">
+            <v>0</v>
           </cell>
         </row>
         <row r="27">
-          <cell r="D27" t="str">
-            <v/>
+          <cell r="D27">
+            <v>0</v>
           </cell>
           <cell r="E27" t="str">
             <v>DATE NATURE２</v>
           </cell>
-          <cell r="F27" t="str">
-            <v/>
+          <cell r="F27">
+            <v>0</v>
           </cell>
           <cell r="G27">
             <v>2</v>
@@ -7468,11 +7483,11 @@
           <cell r="L27">
             <v>0</v>
           </cell>
-          <cell r="N27" t="str">
-            <v/>
-          </cell>
-          <cell r="P27" t="str">
-            <v/>
+          <cell r="N27">
+            <v>0</v>
+          </cell>
+          <cell r="P27">
+            <v>0</v>
           </cell>
           <cell r="R27">
             <v>39800</v>
@@ -7486,43 +7501,43 @@
           <cell r="X27">
             <v>0</v>
           </cell>
-          <cell r="Z27" t="str">
-            <v/>
-          </cell>
-          <cell r="AA27" t="str">
-            <v/>
+          <cell r="Z27">
+            <v>0</v>
+          </cell>
+          <cell r="AA27">
+            <v>0</v>
           </cell>
         </row>
         <row r="28">
-          <cell r="D28" t="str">
-            <v/>
-          </cell>
-          <cell r="E28" t="str">
-            <v/>
-          </cell>
-          <cell r="F28" t="str">
-            <v/>
-          </cell>
-          <cell r="G28" t="str">
-            <v/>
-          </cell>
-          <cell r="H28" t="str">
-            <v/>
+          <cell r="D28">
+            <v>0</v>
+          </cell>
+          <cell r="E28">
+            <v>0</v>
+          </cell>
+          <cell r="F28">
+            <v>0</v>
+          </cell>
+          <cell r="G28">
+            <v>0</v>
+          </cell>
+          <cell r="H28">
+            <v>0</v>
           </cell>
           <cell r="J28">
             <v>0</v>
           </cell>
-          <cell r="L28" t="str">
-            <v/>
-          </cell>
-          <cell r="N28" t="str">
-            <v/>
-          </cell>
-          <cell r="P28" t="str">
-            <v/>
-          </cell>
-          <cell r="R28" t="str">
-            <v/>
+          <cell r="L28">
+            <v>0</v>
+          </cell>
+          <cell r="N28">
+            <v>0</v>
+          </cell>
+          <cell r="P28">
+            <v>0</v>
+          </cell>
+          <cell r="R28">
+            <v>0</v>
           </cell>
           <cell r="T28">
             <v>0</v>
@@ -7533,43 +7548,43 @@
           <cell r="X28">
             <v>0</v>
           </cell>
-          <cell r="Z28" t="str">
-            <v/>
-          </cell>
-          <cell r="AA28" t="str">
-            <v/>
+          <cell r="Z28">
+            <v>0</v>
+          </cell>
+          <cell r="AA28">
+            <v>0</v>
           </cell>
         </row>
         <row r="29">
-          <cell r="D29" t="str">
-            <v/>
-          </cell>
-          <cell r="E29" t="str">
-            <v/>
-          </cell>
-          <cell r="F29" t="str">
-            <v/>
-          </cell>
-          <cell r="G29" t="str">
-            <v/>
-          </cell>
-          <cell r="H29" t="str">
-            <v/>
+          <cell r="D29">
+            <v>0</v>
+          </cell>
+          <cell r="E29">
+            <v>0</v>
+          </cell>
+          <cell r="F29">
+            <v>0</v>
+          </cell>
+          <cell r="G29">
+            <v>0</v>
+          </cell>
+          <cell r="H29">
+            <v>0</v>
           </cell>
           <cell r="J29">
             <v>0</v>
           </cell>
-          <cell r="L29" t="str">
-            <v/>
-          </cell>
-          <cell r="N29" t="str">
-            <v/>
-          </cell>
-          <cell r="P29" t="str">
-            <v/>
-          </cell>
-          <cell r="R29" t="str">
-            <v/>
+          <cell r="L29">
+            <v>0</v>
+          </cell>
+          <cell r="N29">
+            <v>0</v>
+          </cell>
+          <cell r="P29">
+            <v>0</v>
+          </cell>
+          <cell r="R29">
+            <v>0</v>
           </cell>
           <cell r="T29">
             <v>0</v>
@@ -7580,43 +7595,43 @@
           <cell r="X29">
             <v>0</v>
           </cell>
-          <cell r="Z29" t="str">
-            <v/>
-          </cell>
-          <cell r="AA29" t="str">
-            <v/>
+          <cell r="Z29">
+            <v>0</v>
+          </cell>
+          <cell r="AA29">
+            <v>0</v>
           </cell>
         </row>
         <row r="30">
-          <cell r="D30" t="str">
-            <v/>
-          </cell>
-          <cell r="E30" t="str">
-            <v/>
-          </cell>
-          <cell r="F30" t="str">
-            <v/>
-          </cell>
-          <cell r="G30" t="str">
-            <v/>
-          </cell>
-          <cell r="H30" t="str">
-            <v/>
+          <cell r="D30">
+            <v>0</v>
+          </cell>
+          <cell r="E30">
+            <v>0</v>
+          </cell>
+          <cell r="F30">
+            <v>0</v>
+          </cell>
+          <cell r="G30">
+            <v>0</v>
+          </cell>
+          <cell r="H30">
+            <v>0</v>
           </cell>
           <cell r="J30">
             <v>0</v>
           </cell>
-          <cell r="L30" t="str">
-            <v/>
-          </cell>
-          <cell r="N30" t="str">
-            <v/>
-          </cell>
-          <cell r="P30" t="str">
-            <v/>
-          </cell>
-          <cell r="R30" t="str">
-            <v/>
+          <cell r="L30">
+            <v>0</v>
+          </cell>
+          <cell r="N30">
+            <v>0</v>
+          </cell>
+          <cell r="P30">
+            <v>0</v>
+          </cell>
+          <cell r="R30">
+            <v>0</v>
           </cell>
           <cell r="T30">
             <v>0</v>
@@ -7627,43 +7642,43 @@
           <cell r="X30">
             <v>0</v>
           </cell>
-          <cell r="Z30" t="str">
-            <v/>
-          </cell>
-          <cell r="AA30" t="str">
-            <v/>
+          <cell r="Z30">
+            <v>0</v>
+          </cell>
+          <cell r="AA30">
+            <v>0</v>
           </cell>
         </row>
         <row r="31">
-          <cell r="D31" t="str">
-            <v/>
-          </cell>
-          <cell r="E31" t="str">
-            <v/>
-          </cell>
-          <cell r="F31" t="str">
-            <v/>
-          </cell>
-          <cell r="G31" t="str">
-            <v/>
-          </cell>
-          <cell r="H31" t="str">
-            <v/>
+          <cell r="D31">
+            <v>0</v>
+          </cell>
+          <cell r="E31">
+            <v>0</v>
+          </cell>
+          <cell r="F31">
+            <v>0</v>
+          </cell>
+          <cell r="G31">
+            <v>0</v>
+          </cell>
+          <cell r="H31">
+            <v>0</v>
           </cell>
           <cell r="J31">
             <v>0</v>
           </cell>
-          <cell r="L31" t="str">
-            <v/>
-          </cell>
-          <cell r="N31" t="str">
-            <v/>
-          </cell>
-          <cell r="P31" t="str">
-            <v/>
-          </cell>
-          <cell r="R31" t="str">
-            <v/>
+          <cell r="L31">
+            <v>0</v>
+          </cell>
+          <cell r="N31">
+            <v>0</v>
+          </cell>
+          <cell r="P31">
+            <v>0</v>
+          </cell>
+          <cell r="R31">
+            <v>0</v>
           </cell>
           <cell r="T31">
             <v>0</v>
@@ -7674,43 +7689,43 @@
           <cell r="X31">
             <v>0</v>
           </cell>
-          <cell r="Z31" t="str">
-            <v/>
-          </cell>
-          <cell r="AA31" t="str">
-            <v/>
+          <cell r="Z31">
+            <v>0</v>
+          </cell>
+          <cell r="AA31">
+            <v>0</v>
           </cell>
         </row>
         <row r="32">
-          <cell r="D32" t="str">
-            <v/>
-          </cell>
-          <cell r="E32" t="str">
-            <v/>
-          </cell>
-          <cell r="F32" t="str">
-            <v/>
-          </cell>
-          <cell r="G32" t="str">
-            <v/>
-          </cell>
-          <cell r="H32" t="str">
-            <v/>
+          <cell r="D32">
+            <v>0</v>
+          </cell>
+          <cell r="E32">
+            <v>0</v>
+          </cell>
+          <cell r="F32">
+            <v>0</v>
+          </cell>
+          <cell r="G32">
+            <v>0</v>
+          </cell>
+          <cell r="H32">
+            <v>0</v>
           </cell>
           <cell r="J32">
             <v>0</v>
           </cell>
-          <cell r="L32" t="str">
-            <v/>
-          </cell>
-          <cell r="N32" t="str">
-            <v/>
-          </cell>
-          <cell r="P32" t="str">
-            <v/>
-          </cell>
-          <cell r="R32" t="str">
-            <v/>
+          <cell r="L32">
+            <v>0</v>
+          </cell>
+          <cell r="N32">
+            <v>0</v>
+          </cell>
+          <cell r="P32">
+            <v>0</v>
+          </cell>
+          <cell r="R32">
+            <v>0</v>
           </cell>
           <cell r="T32">
             <v>0</v>
@@ -7721,43 +7736,43 @@
           <cell r="X32">
             <v>0</v>
           </cell>
-          <cell r="Z32" t="str">
-            <v/>
-          </cell>
-          <cell r="AA32" t="str">
-            <v/>
+          <cell r="Z32">
+            <v>0</v>
+          </cell>
+          <cell r="AA32">
+            <v>0</v>
           </cell>
         </row>
         <row r="33">
-          <cell r="D33" t="str">
-            <v/>
-          </cell>
-          <cell r="E33" t="str">
-            <v/>
-          </cell>
-          <cell r="F33" t="str">
-            <v/>
-          </cell>
-          <cell r="G33" t="str">
-            <v/>
-          </cell>
-          <cell r="H33" t="str">
-            <v/>
+          <cell r="D33">
+            <v>0</v>
+          </cell>
+          <cell r="E33">
+            <v>0</v>
+          </cell>
+          <cell r="F33">
+            <v>0</v>
+          </cell>
+          <cell r="G33">
+            <v>0</v>
+          </cell>
+          <cell r="H33">
+            <v>0</v>
           </cell>
           <cell r="J33">
             <v>0</v>
           </cell>
-          <cell r="L33" t="str">
-            <v/>
-          </cell>
-          <cell r="N33" t="str">
-            <v/>
-          </cell>
-          <cell r="P33" t="str">
-            <v/>
-          </cell>
-          <cell r="R33" t="str">
-            <v/>
+          <cell r="L33">
+            <v>0</v>
+          </cell>
+          <cell r="N33">
+            <v>0</v>
+          </cell>
+          <cell r="P33">
+            <v>0</v>
+          </cell>
+          <cell r="R33">
+            <v>0</v>
           </cell>
           <cell r="T33">
             <v>0</v>
@@ -7768,43 +7783,43 @@
           <cell r="X33">
             <v>0</v>
           </cell>
-          <cell r="Z33" t="str">
-            <v/>
-          </cell>
-          <cell r="AA33" t="str">
-            <v/>
+          <cell r="Z33">
+            <v>0</v>
+          </cell>
+          <cell r="AA33">
+            <v>0</v>
           </cell>
         </row>
         <row r="34">
-          <cell r="D34" t="str">
-            <v/>
-          </cell>
-          <cell r="E34" t="str">
-            <v/>
-          </cell>
-          <cell r="F34" t="str">
-            <v/>
-          </cell>
-          <cell r="G34" t="str">
-            <v/>
-          </cell>
-          <cell r="H34" t="str">
-            <v/>
+          <cell r="D34">
+            <v>0</v>
+          </cell>
+          <cell r="E34">
+            <v>0</v>
+          </cell>
+          <cell r="F34">
+            <v>0</v>
+          </cell>
+          <cell r="G34">
+            <v>0</v>
+          </cell>
+          <cell r="H34">
+            <v>0</v>
           </cell>
           <cell r="J34">
             <v>0</v>
           </cell>
-          <cell r="L34" t="str">
-            <v/>
-          </cell>
-          <cell r="N34" t="str">
-            <v/>
-          </cell>
-          <cell r="P34" t="str">
-            <v/>
-          </cell>
-          <cell r="R34" t="str">
-            <v/>
+          <cell r="L34">
+            <v>0</v>
+          </cell>
+          <cell r="N34">
+            <v>0</v>
+          </cell>
+          <cell r="P34">
+            <v>0</v>
+          </cell>
+          <cell r="R34">
+            <v>0</v>
           </cell>
           <cell r="T34">
             <v>0</v>
@@ -7815,11 +7830,11 @@
           <cell r="X34">
             <v>0</v>
           </cell>
-          <cell r="Z34" t="str">
-            <v/>
-          </cell>
-          <cell r="AA34" t="str">
-            <v/>
+          <cell r="Z34">
+            <v>0</v>
+          </cell>
+          <cell r="AA34">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -8287,7 +8302,9 @@
             <v>FT2400 ﾓﾃﾞﾙ 6200-40N</v>
           </cell>
           <cell r="E6" t="str">
-            <v>PentiumPro-200､ﾒﾓﾘ:64MB､HDD:4GB､最大16倍速CD-ROM､100BASE-TX､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､WindowsNT Server 4.0(10ｸﾗｲｱﾝﾄﾗｲｾﾝｽ付き)ﾌﾟﾘｲﾝｽﾄｰﾙ､ｻｰﾊﾞ管理ｿﾌﾄｳｪｱﾊﾞﾝﾄﾞﾙ</v>
+            <v>PentiumPro-200､ﾒﾓﾘ:64MB､HDD:4GB､最大16倍速CD-ROM､
+100BASE-TX､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､WindowsNT Server 4.0
+(10ｸﾗｲｱﾝﾄﾗｲｾﾝｽ付き)ﾌﾟﾘｲﾝｽﾄｰﾙ､ｻｰﾊﾞ管理ｿﾌﾄｳｪｱﾊﾞﾝﾄﾞﾙ</v>
           </cell>
           <cell r="F6">
             <v>1318000</v>
@@ -8451,7 +8468,8 @@
             <v>FT2400 ﾓﾃﾞﾙ 6200-40</v>
           </cell>
           <cell r="E7" t="str">
-            <v>PentiumPro-200､ﾒﾓﾘ:64MB､HDD:4GB､最大16倍速CD-ROM､100BASE-TX､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､ｻｰﾊﾞ管理ｿﾌﾄｳｪｱﾊﾞﾝﾄﾞﾙ</v>
+            <v>PentiumPro-200､ﾒﾓﾘ:64MB､HDD:4GB､最大16倍速CD-ROM､
+100BASE-TX､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､ｻｰﾊﾞ管理ｿﾌﾄｳｪｱﾊﾞﾝﾄﾞﾙ</v>
           </cell>
           <cell r="F7">
             <v>1158000</v>
@@ -8943,7 +8961,8 @@
             <v>FT1200 ﾓﾃﾞﾙ 6200-40N</v>
           </cell>
           <cell r="E10" t="str">
-            <v>PentiumPro-200､ﾒﾓﾘ:32MB､HDD:4GB､8倍速CD-ROM､100BASE-TX､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､WindowsNT Server 4.0(10ｸﾗｲｱﾝﾄﾗｲｾﾝｽ付き)ﾌﾟﾘｲﾝｽﾄｰﾙ</v>
+            <v>PentiumPro-200､ﾒﾓﾘ:32MB､HDD:4GB､8倍速CD-ROM､100BASE-TX､
+ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､WindowsNT Server 4.0(10ｸﾗｲｱﾝﾄﾗｲｾﾝｽ付き)ﾌﾟﾘｲﾝｽﾄｰﾙ</v>
           </cell>
           <cell r="F10">
             <v>758000</v>
@@ -9107,7 +9126,8 @@
             <v>FT1200 ﾓﾃﾞﾙ 6200-40</v>
           </cell>
           <cell r="E11" t="str">
-            <v>PentiumPro-200､ﾒﾓﾘ:32MB､HDD:4GB､8倍速CD-ROM､100BASE-TX､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ</v>
+            <v>PentiumPro-200､ﾒﾓﾘ:32MB､HDD:4GB､8倍速CD-ROM､100BASE-TX､
+ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ</v>
           </cell>
           <cell r="F11">
             <v>598000</v>
@@ -9271,7 +9291,8 @@
             <v>FT1200 ﾓﾃﾞﾙ 6200-20N</v>
           </cell>
           <cell r="E12" t="str">
-            <v>PentiumPro-200､ﾒﾓﾘ:32MB､HDD:2GB､8倍速CD-ROM､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､WindowsNT Server 4.0(10ｸﾗｲｱﾝﾄﾗｲｾﾝｽ付き)ﾌﾟﾘｲﾝｽﾄｰﾙ</v>
+            <v>PentiumPro-200､ﾒﾓﾘ:32MB､HDD:2GB､8倍速CD-ROM､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､
+WindowsNT Server 4.0(10ｸﾗｲｱﾝﾄﾗｲｾﾝｽ付き)ﾌﾟﾘｲﾝｽﾄｰﾙ</v>
           </cell>
           <cell r="F12">
             <v>758000</v>
@@ -9602,7 +9623,8 @@
             <v>････</v>
           </cell>
           <cell r="D14" t="str">
-            <v>apricot PCｻ-ﾊﾞH/Wｺﾝﾌｨｸﾞﾚ-ｼｮﾝｻ-ﾋﾞｽ</v>
+            <v>apricot PCｻ-ﾊﾞ
+H/Wｺﾝﾌｨｸﾞﾚ-ｼｮﾝｻ-ﾋﾞｽ</v>
           </cell>
           <cell r="E14" t="str">
             <v>RAIDを増設する場合｡増設するH/Wの品目数に制限なし｡</v>
@@ -9766,7 +9788,8 @@
             <v>････</v>
           </cell>
           <cell r="D15" t="str">
-            <v>apricot PCｻ-ﾊﾞH/Wｺﾝﾌｨｸﾞﾚ-ｼｮﾝｻ-ﾋﾞｽ</v>
+            <v>apricot PCｻ-ﾊﾞ
+H/Wｺﾝﾌｨｸﾞﾚ-ｼｮﾝｻ-ﾋﾞｽ</v>
           </cell>
           <cell r="E15" t="str">
             <v>RAIDを増設しない場合｡増設するH/Wの品目数は4品目以上｡</v>
@@ -9930,7 +9953,8 @@
             <v>････</v>
           </cell>
           <cell r="D16" t="str">
-            <v>apricot PCｻ-ﾊﾞH/Wｺﾝﾌｨｸﾞﾚ-ｼｮﾝｻ-ﾋﾞｽ</v>
+            <v>apricot PCｻ-ﾊﾞ
+H/Wｺﾝﾌｨｸﾞﾚ-ｼｮﾝｻ-ﾋﾞｽ</v>
           </cell>
           <cell r="E16" t="str">
             <v>RAIDを増設しない場合｡増設するH/Wの品目数は3品目以下｡</v>
@@ -10102,7 +10126,8 @@
             <v>LS550 ﾓﾃﾞﾙ 6200-32MCN</v>
           </cell>
           <cell r="E18" t="str">
-            <v>PentiumPro-200､ﾒﾓﾘ:32MB､HDD:3.2GB､8倍速CD-ROM､100BASE-TX､ｻｳﾝﾄﾞ機能､ｷ-ﾎﾞ-ﾄﾞ､ﾏｳｽ､WindowsNT Workstation 4.0ﾌﾟﾘｲﾝｽﾄｰﾙ</v>
+            <v>PentiumPro-200､ﾒﾓﾘ:32MB､HDD:3.2GB､8倍速CD-ROM､100BASE-TX､
+ｻｳﾝﾄﾞ機能､ｷ-ﾎﾞ-ﾄﾞ､ﾏｳｽ､WindowsNT Workstation 4.0ﾌﾟﾘｲﾝｽﾄｰﾙ</v>
           </cell>
           <cell r="F18">
             <v>498000</v>
@@ -10266,7 +10291,8 @@
             <v>LS660 ﾓﾃﾞﾙ 5200M-21CX</v>
           </cell>
           <cell r="E19" t="str">
-            <v>MMXﾃｸﾉﾛｼﾞPentium-200､ﾒﾓﾘ:16MB､HDD:2.1GB､8倍速CD-ROM､100BASE-TX､ｻｳﾝﾄﾞ機能､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､Windows95</v>
+            <v>MMXﾃｸﾉﾛｼﾞPentium-200､ﾒﾓﾘ:16MB､HDD:2.1GB､8倍速CD-ROM､
+100BASE-TX､ｻｳﾝﾄﾞ機能､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､Windows95</v>
           </cell>
           <cell r="F19">
             <v>348000</v>
@@ -10430,7 +10456,8 @@
             <v>LS660 ﾓﾃﾞﾙ 5166-21CX</v>
           </cell>
           <cell r="E20" t="str">
-            <v>Pentium-166､ﾒﾓﾘ:16MB､HDD:2.1GB､8倍速CD-ROM､10BASE-T/2/5､ｻｳﾝﾄﾞ機能､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､Windows95</v>
+            <v>Pentium-166､ﾒﾓﾘ:16MB､HDD:2.1GB､8倍速CD-ROM､10BASE-T/2/5､
+ｻｳﾝﾄﾞ機能､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､Windows95</v>
           </cell>
           <cell r="F20">
             <v>338000</v>
@@ -10761,7 +10788,8 @@
             <v>LS550 ﾓﾃﾞﾙ 5200-32CX</v>
           </cell>
           <cell r="E22" t="str">
-            <v>Pentium-200､ﾒﾓﾘ:16MB､HDD:3.2GB､8倍速CD-ROM､10BASE-T/2/5､ｻｳﾝﾄﾞ機能､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､Windows95</v>
+            <v>Pentium-200､ﾒﾓﾘ:16MB､HDD:3.2GB､8倍速CD-ROM､10BASE-T/2/5､
+ｻｳﾝﾄﾞ機能､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､Windows95</v>
           </cell>
           <cell r="F22">
             <v>428000</v>
@@ -10928,7 +10956,8 @@
             <v>LS550 ﾓﾃﾞﾙ 5200-32CW</v>
           </cell>
           <cell r="E23" t="str">
-            <v>Pentium-200､ﾒﾓﾘ:16MB､HDD:3.2GB､8倍速CD-ROM､ｻｳﾝﾄﾞ機能､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､Windows3.1</v>
+            <v>Pentium-200､ﾒﾓﾘ:16MB､HDD:3.2GB､8倍速CD-ROM､ｻｳﾝﾄﾞ機能､
+ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､Windows3.1</v>
           </cell>
           <cell r="F23">
             <v>423000</v>
@@ -11095,7 +11124,8 @@
             <v>LS550 ﾓﾃﾞﾙ 5200M-21CX</v>
           </cell>
           <cell r="E24" t="str">
-            <v>MMXﾃｸﾉﾛｼﾞPentium-200､ﾒﾓﾘ:16MB､HDD:2.1GB､8倍速CD-ROM､100BASE-TX､ｻｳﾝﾄﾞ機能､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､Windows95</v>
+            <v>MMXﾃｸﾉﾛｼﾞPentium-200､ﾒﾓﾘ:16MB､HDD:2.1GB､8倍速CD-ROM､
+100BASE-TX､ｻｳﾝﾄﾞ機能､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､Windows95</v>
           </cell>
           <cell r="F24">
             <v>328000</v>
@@ -11259,7 +11289,8 @@
             <v>LS550 ﾓﾃﾞﾙ 5166-21CX　</v>
           </cell>
           <cell r="E25" t="str">
-            <v>Pentium-166､ﾒﾓﾘ:16MB､HDD:2.1GB､8倍速CD-ROM､10BASE-T/2/5､ｻｳﾝﾄﾞ機能､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､Windows95</v>
+            <v>Pentium-166､ﾒﾓﾘ:16MB､HDD:2.1GB､8倍速CD-ROM､10BASE-T/2/5､
+ｻｳﾝﾄﾞ機能､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､Windows95</v>
           </cell>
           <cell r="F25">
             <v>328000</v>
@@ -11426,7 +11457,8 @@
             <v>LS550 ﾓﾃﾞﾙ 5166-21CW</v>
           </cell>
           <cell r="E26" t="str">
-            <v>Pentium-166､ﾒﾓﾘ:16MB､HDD:2.1GB､8倍速CD-ROM､ｻｳﾝﾄﾞ機能､ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､Windows3.1</v>
+            <v>Pentium-166､ﾒﾓﾘ:16MB､HDD:2.1GB､8倍速CD-ROM､ｻｳﾝﾄﾞ機能､
+ｷｰﾎﾞｰﾄﾞ､ﾏｳｽ､Windows3.1</v>
           </cell>
           <cell r="F26">
             <v>323000</v>
@@ -12251,13 +12283,18 @@
             <v>ACN-35-AL1</v>
           </cell>
           <cell r="C32" t="str">
-            <v>M3435-A1C03C589D-TP</v>
+            <v>M3435-A1C0
+3C589D-TP</v>
           </cell>
           <cell r="D32" t="str">
-            <v>apricotNOTE ALﾓﾃﾞﾙ 5150M-14TXLANｾｯﾄﾓﾃﾞﾙ</v>
+            <v>apricotNOTE AL
+ﾓﾃﾞﾙ 5150M-14TX
+LANｾｯﾄﾓﾃﾞﾙ</v>
           </cell>
           <cell r="E32" t="str">
-            <v>MMXﾃｸﾉﾛｼﾞPentium-150､ﾒﾓﾘ:32MB､HDD:1.44GB､12.1ｲﾝﾁTFTｶﾗｰ(1024*768)､Windows95､3Com社製LANｱﾀﾞﾌﾟﾀ(10BASE-T)付き</v>
+            <v>MMXﾃｸﾉﾛｼﾞPentium-150､ﾒﾓﾘ:32MB､HDD:1.44GB､
+12.1ｲﾝﾁTFTｶﾗｰ(1024*768)､Windows95､
+3Com社製LANｱﾀﾞﾌﾟﾀ(10BASE-T)付き</v>
           </cell>
           <cell r="F32">
             <v>558000</v>
@@ -12415,13 +12452,18 @@
             <v>ACN-35-AL2</v>
           </cell>
           <cell r="C33" t="str">
-            <v>M3435-A2C03C589D-TP</v>
+            <v>M3435-A2C0
+3C589D-TP</v>
           </cell>
           <cell r="D33" t="str">
-            <v>apricotNOTE ALﾓﾃﾞﾙ 5133M-14TXLANｾｯﾄﾓﾃﾞﾙ</v>
+            <v>apricotNOTE AL
+ﾓﾃﾞﾙ 5133M-14TX
+LANｾｯﾄﾓﾃﾞﾙ</v>
           </cell>
           <cell r="E33" t="str">
-            <v>MMXﾃｸﾉﾛｼﾞPentium-133､ﾒﾓﾘ:16MB､HDD:1.44GB､12.1ｲﾝﾁTFTｶﾗｰ(800*600)､Windows95､3Com社製LANｱﾀﾞﾌﾟﾀ(10BASE-T)付き</v>
+            <v>MMXﾃｸﾉﾛｼﾞPentium-133､ﾒﾓﾘ:16MB､HDD:1.44GB､
+12.1ｲﾝﾁTFTｶﾗｰ(800*600)､Windows95､
+3Com社製LANｱﾀﾞﾌﾟﾀ(10BASE-T)付き</v>
           </cell>
           <cell r="F33">
             <v>458000</v>
@@ -12582,10 +12624,12 @@
             <v>M3435-A1C0</v>
           </cell>
           <cell r="D34" t="str">
-            <v>apricotNOTE ALﾓﾃﾞﾙ 5150M-14TX</v>
+            <v>apricotNOTE AL
+ﾓﾃﾞﾙ 5150M-14TX</v>
           </cell>
           <cell r="E34" t="str">
-            <v>MMXﾃｸﾉﾛｼﾞPentium-150､ﾒﾓﾘ:32MB､HDD:1.44GB､12.1ｲﾝﾁTFTｶﾗｰ(1024*768)､Windows95</v>
+            <v>MMXﾃｸﾉﾛｼﾞPentium-150､ﾒﾓﾘ:32MB､HDD:1.44GB､
+12.1ｲﾝﾁTFTｶﾗｰ(1024*768)､Windows95</v>
           </cell>
           <cell r="F34">
             <v>538000</v>
@@ -12746,10 +12790,12 @@
             <v>M3435-A2C0</v>
           </cell>
           <cell r="D35" t="str">
-            <v>apricotNOTE ALﾓﾃﾞﾙ 5133M-14TX</v>
+            <v>apricotNOTE AL
+ﾓﾃﾞﾙ 5133M-14TX</v>
           </cell>
           <cell r="E35" t="str">
-            <v>MMXﾃｸﾉﾛｼﾞPentium-133､ﾒﾓﾘ:16MB､HDD:1.44GB､12.1ｲﾝﾁTFTｶﾗｰ(800*600)､Windows95</v>
+            <v>MMXﾃｸﾉﾛｼﾞPentium-133､ﾒﾓﾘ:16MB､HDD:1.44GB､
+12.1ｲﾝﾁTFTｶﾗｰ(800*600)､Windows95</v>
           </cell>
           <cell r="F35">
             <v>438000</v>
@@ -12907,13 +12953,17 @@
             <v>ACN-45-AL1</v>
           </cell>
           <cell r="C36" t="str">
-            <v>M3445-A1C03C589D-TP</v>
+            <v>M3445-A1C0
+3C589D-TP</v>
           </cell>
           <cell r="D36" t="str">
-            <v>apricotNOTE ELﾓﾃﾞﾙ 5150-14TXLANｾｯﾄﾓﾃﾞﾙ</v>
+            <v>apricotNOTE EL
+ﾓﾃﾞﾙ 5150-14TX
+LANｾｯﾄﾓﾃﾞﾙ</v>
           </cell>
           <cell r="E36" t="str">
-            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁTFTｶﾗｰ(800*600)､Windows95､3Com社製LANｱﾀﾞﾌﾟﾀ(10BASE-T)付き</v>
+            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁTFTｶﾗｰ(800*600)､
+Windows95､3Com社製LANｱﾀﾞﾌﾟﾀ(10BASE-T)付き</v>
           </cell>
           <cell r="F36">
             <v>378000</v>
@@ -13071,13 +13121,18 @@
             <v>ACN-45-AL2</v>
           </cell>
           <cell r="C37" t="str">
-            <v>M3445-A2C03C589D-TP</v>
+            <v>M3445-A2C0
+3C589D-TP</v>
           </cell>
           <cell r="D37" t="str">
-            <v>apricotNOTE ELﾓﾃﾞﾙ 5150-14DXLANｾｯﾄﾓﾃﾞﾙ</v>
+            <v>apricotNOTE EL
+ﾓﾃﾞﾙ 5150-14DX
+LANｾｯﾄﾓﾃﾞﾙ</v>
           </cell>
           <cell r="E37" t="str">
-            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁASA方式DSTNｶﾗｰ(800*600)､Windows95､3Com社製LANｱﾀﾞﾌﾟﾀ(10BASE-T)付き</v>
+            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:1.44GB､
+11.3ｲﾝﾁASA方式DSTNｶﾗｰ(800*600)､Windows95､
+3Com社製LANｱﾀﾞﾌﾟﾀ(10BASE-T)付き</v>
           </cell>
           <cell r="F37">
             <v>308000</v>
@@ -13235,13 +13290,18 @@
             <v>ACN-45-AL2W</v>
           </cell>
           <cell r="C38" t="str">
-            <v>M3445-A2W03C589D-TP</v>
+            <v>M3445-A2W0
+3C589D-TP</v>
           </cell>
           <cell r="D38" t="str">
-            <v>apricotNOTE ELﾓﾃﾞﾙ 5150-14DWLANｾｯﾄﾓﾃﾞﾙ</v>
+            <v>apricotNOTE EL
+ﾓﾃﾞﾙ 5150-14DW
+LANｾｯﾄﾓﾃﾞﾙ</v>
           </cell>
           <cell r="E38" t="str">
-            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁASA方式DSTNｶﾗｰ(800*600)､Windows3.1､3Com社製LANｱﾀﾞﾌﾟﾀ(10BASE-T)付き</v>
+            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:1.44GB､
+11.3ｲﾝﾁASA方式DSTNｶﾗｰ(800*600)､Windows3.1､
+3Com社製LANｱﾀﾞﾌﾟﾀ(10BASE-T)付き</v>
           </cell>
           <cell r="F38">
             <v>318000</v>
@@ -13402,10 +13462,12 @@
             <v>M3445-A1C0</v>
           </cell>
           <cell r="D39" t="str">
-            <v>apricotNOTE ELﾓﾃﾞﾙ 5150-14TX</v>
+            <v>apricotNOTE EL
+ﾓﾃﾞﾙ 5150-14TX</v>
           </cell>
           <cell r="E39" t="str">
-            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁTFTｶﾗｰ(800*600)､Windows95</v>
+            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁTFTｶﾗｰ(800*600)､
+Windows95</v>
           </cell>
           <cell r="F39">
             <v>358000</v>
@@ -13566,10 +13628,12 @@
             <v>M3445-A2C0</v>
           </cell>
           <cell r="D40" t="str">
-            <v>apricotNOTE ELﾓﾃﾞﾙ 5150-14DX</v>
+            <v>apricotNOTE EL
+ﾓﾃﾞﾙ 5150-14DX</v>
           </cell>
           <cell r="E40" t="str">
-            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁASA方式DSTNｶﾗｰ(800*600)､Windows95</v>
+            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:1.44GB､
+11.3ｲﾝﾁASA方式DSTNｶﾗｰ(800*600)､Windows95</v>
           </cell>
           <cell r="F40">
             <v>288000</v>
@@ -13730,10 +13794,12 @@
             <v>M3445-A2W0</v>
           </cell>
           <cell r="D41" t="str">
-            <v>apricotNOTE ELﾓﾃﾞﾙ 5150-14DW</v>
+            <v>apricotNOTE EL
+ﾓﾃﾞﾙ 5150-14DW</v>
           </cell>
           <cell r="E41" t="str">
-            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁASA方式DSTNｶﾗｰ(800*600)､Windows3.1</v>
+            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:1.44GB､
+11.3ｲﾝﾁASA方式DSTNｶﾗｰ(800*600)､Windows3.1</v>
           </cell>
           <cell r="F41">
             <v>298000</v>
@@ -13894,10 +13960,12 @@
             <v>M3423-C3C0</v>
           </cell>
           <cell r="D42" t="str">
-            <v>apricotNOTE SXﾓﾃﾞﾙ 5166M-21TX</v>
+            <v>apricotNOTE SX
+ﾓﾃﾞﾙ 5166M-21TX</v>
           </cell>
           <cell r="E42" t="str">
-            <v>MMXﾃｸﾉﾛｼﾞPentium-166､ﾒﾓﾘ:16MB､HDD:2.1GB､12.1ｲﾝﾁTFTｶﾗｰ(1024*768)､DSVD対応FAXﾓﾃﾞﾑ､Windows95</v>
+            <v>MMXﾃｸﾉﾛｼﾞPentium-166､ﾒﾓﾘ:16MB､HDD:2.1GB､
+12.1ｲﾝﾁTFTｶﾗｰ(1024*768)､DSVD対応FAXﾓﾃﾞﾑ､Windows95</v>
           </cell>
           <cell r="F42">
             <v>698000</v>
@@ -14058,10 +14126,12 @@
             <v>M3484-C1C0</v>
           </cell>
           <cell r="D43" t="str">
-            <v>apricotNOTE FXﾓﾃﾞﾙ 5150-21X</v>
+            <v>apricotNOTE FX
+ﾓﾃﾞﾙ 5150-21X</v>
           </cell>
           <cell r="E43" t="str">
-            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:2.1GB､12.1ｲﾝﾁTFTｶﾗｰ(800*600)､Windows95</v>
+            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:2.1GB､12.1ｲﾝﾁTFTｶﾗｰ(800*600)､
+Windows95</v>
           </cell>
           <cell r="F43">
             <v>548000</v>
@@ -14225,10 +14295,12 @@
             <v>M3484-C1W0</v>
           </cell>
           <cell r="D44" t="str">
-            <v>apricotNOTE FXﾓﾃﾞﾙ 5150-21W</v>
+            <v>apricotNOTE FX
+ﾓﾃﾞﾙ 5150-21W</v>
           </cell>
           <cell r="E44" t="str">
-            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:2.1GB､12.1ｲﾝﾁTFTｶﾗｰ(800*600)､Windows3.1</v>
+            <v>Pentium-150､ﾒﾓﾘ:16MB､HDD:2.1GB､12.1ｲﾝﾁTFTｶﾗｰ(800*600)､
+Windows3.1</v>
           </cell>
           <cell r="F44">
             <v>548000</v>
@@ -14261,7 +14333,8 @@
             <v>AC</v>
           </cell>
           <cell r="P44" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q44">
             <v>0</v>
@@ -14381,7 +14454,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD44" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="45">
@@ -14392,10 +14466,12 @@
             <v>M3464-D3C0</v>
           </cell>
           <cell r="D45" t="str">
-            <v>apricotNOTE GXﾓﾃﾞﾙ 5133-14DX</v>
+            <v>apricotNOTE GX
+ﾓﾃﾞﾙ 5133-14DX</v>
           </cell>
           <cell r="E45" t="str">
-            <v>Pentium-133､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁDSTNｶﾗｰ(800*600)､Windows95</v>
+            <v>Pentium-133､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁDSTNｶﾗｰ(800*600)､
+Windows95</v>
           </cell>
           <cell r="F45">
             <v>318000</v>
@@ -14428,7 +14504,8 @@
             <v>AC</v>
           </cell>
           <cell r="P45" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q45">
             <v>0</v>
@@ -14548,7 +14625,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD45" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="46">
@@ -14559,10 +14637,12 @@
             <v>M3464-D3W0</v>
           </cell>
           <cell r="D46" t="str">
-            <v>apricotNOTE GXﾓﾃﾞﾙ 5133-14DW</v>
+            <v>apricotNOTE GX
+ﾓﾃﾞﾙ 5133-14DW</v>
           </cell>
           <cell r="E46" t="str">
-            <v>Pentium-133､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁDSTNｶﾗｰ(800*600)､Windows3.1</v>
+            <v>Pentium-133､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁDSTNｶﾗｰ(800*600)､
+Windows3.1</v>
           </cell>
           <cell r="F46">
             <v>318000</v>
@@ -14726,10 +14806,12 @@
             <v>M3464-D2C0</v>
           </cell>
           <cell r="D47" t="str">
-            <v>apricotNOTE GXﾓﾃﾞﾙ 5133-14X</v>
+            <v>apricotNOTE GX
+ﾓﾃﾞﾙ 5133-14X</v>
           </cell>
           <cell r="E47" t="str">
-            <v>Pentium-133､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁTFTｶﾗｰ(800*600)､Windows95</v>
+            <v>Pentium-133､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁTFTｶﾗｰ(800*600)､
+Windows95</v>
           </cell>
           <cell r="F47">
             <v>378000</v>
@@ -14893,10 +14975,12 @@
             <v>M3464-D2W0</v>
           </cell>
           <cell r="D48" t="str">
-            <v>apricotNOTE GXﾓﾃﾞﾙ 5133-14W</v>
+            <v>apricotNOTE GX
+ﾓﾃﾞﾙ 5133-14W</v>
           </cell>
           <cell r="E48" t="str">
-            <v>Pentium-133､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁTFTｶﾗｰ(800*600)､Windows3.1</v>
+            <v>Pentium-133､ﾒﾓﾘ:16MB､HDD:1.44GB､11.3ｲﾝﾁTFTｶﾗｰ(800*600)､
+Windows3.1</v>
           </cell>
           <cell r="F48">
             <v>378000</v>
@@ -15060,10 +15144,12 @@
             <v>M3464-D1C0</v>
           </cell>
           <cell r="D49" t="str">
-            <v>apricotNOTE GXﾓﾃﾞﾙ 5120-14X</v>
+            <v>apricotNOTE GX
+ﾓﾃﾞﾙ 5120-14X</v>
           </cell>
           <cell r="E49" t="str">
-            <v>Pentium-120､ﾒﾓﾘ:16MB､HDD:1.08GB､11.3ｲﾝﾁDSTNｶﾗｰ(800*600)､Windows95</v>
+            <v>Pentium-120､ﾒﾓﾘ:16MB､HDD:1.08GB､11.3ｲﾝﾁDSTNｶﾗｰ(800*600)､
+Windows95</v>
           </cell>
           <cell r="F49">
             <v>328000</v>
@@ -15227,10 +15313,12 @@
             <v>M3464-D1W0</v>
           </cell>
           <cell r="D50" t="str">
-            <v>apricotNOTE GXﾓﾃﾞﾙ 5120-14W</v>
+            <v>apricotNOTE GX
+ﾓﾃﾞﾙ 5120-14W</v>
           </cell>
           <cell r="E50" t="str">
-            <v>Pentium-120､ﾒﾓﾘ:16MB､HDD:1.08GB､11.3ｲﾝﾁDSTNｶﾗｰ(800*600)､Windows3.1</v>
+            <v>Pentium-120､ﾒﾓﾘ:16MB､HDD:1.08GB､11.3ｲﾝﾁDSTNｶﾗｰ(800*600)､
+Windows3.1</v>
           </cell>
           <cell r="F50">
             <v>328000</v>
@@ -16717,7 +16805,9 @@
             <v>4MB増設ﾒﾓﾘｷｯﾄ</v>
           </cell>
           <cell r="E60" t="str">
-            <v>LS550(M3551-A/B/Cﾓﾃﾞﾙ､M3553-Aﾓﾃﾞﾙ､M3554-Aﾓﾃﾞﾙ)､XEN-PC､XEN-LSⅡ用｡4MB(SIMM)×1個｡但し､CPUがPentiumの場合は同じ容量のﾒﾓﾘを2個ずつ増設する必要あり｡</v>
+            <v>LS550(M3551-A/B/Cﾓﾃﾞﾙ､M3553-Aﾓﾃﾞﾙ､M3554-Aﾓﾃﾞﾙ)､XEN-PC､
+XEN-LSⅡ用｡4MB(SIMM)×1個｡但し､CPUがPentiumの場合は同じ容量
+のﾒﾓﾘを2個ずつ増設する必要あり｡</v>
           </cell>
           <cell r="F60" t="str">
             <v>OPEN価格</v>
@@ -16881,7 +16971,10 @@
             <v>8MB増設ﾒﾓﾘｷｯﾄ</v>
           </cell>
           <cell r="E61" t="str">
-            <v>FT//ex(M3517､M3518､M3519､M3520､M3521)､LS550(M3551-A/B/Cﾓﾃﾞﾙ､M3553-Aﾓﾃﾞﾙ､M3554-Aﾓﾃﾞﾙ)､XEN-PC､XEN-LSⅡ用｡4MB(SIMM)×1個｡但し､CPUがPentiumの場合は同じ容量のﾒﾓﾘを2個ずつ増設する必要あり｡</v>
+            <v>FT//ex(M3517､M3518､M3519､M3520､M3521)､
+LS550(M3551-A/B/Cﾓﾃﾞﾙ､M3553-Aﾓﾃﾞﾙ､M3554-Aﾓﾃﾞﾙ)､XEN-PC､
+XEN-LSⅡ用｡4MB(SIMM)×1個｡但し､CPUがPentiumの場合は同じ容量
+のﾒﾓﾘを2個ずつ増設する必要あり｡</v>
           </cell>
           <cell r="F61">
             <v>60000</v>
@@ -17048,7 +17141,10 @@
             <v>8MB増設ﾒﾓﾘｷｯﾄ</v>
           </cell>
           <cell r="E62" t="str">
-            <v>FT//ex(M3517､M3518､M3519､M3520､M3521)､LS550(M3551-A/B/Cﾓﾃﾞﾙ､M3553-Aﾓﾃﾞﾙ､M3554-Aﾓﾃﾞﾙ)､XEN-PC(M3456-Cﾓﾃﾞﾙ､M3466-Bﾓﾃﾞﾙ､M3476-Aﾓﾃﾞﾙ)用｡但し､CPUがPentiumの場合は同じ容量のﾒﾓﾘを2個ずつ増設する必要あり｡</v>
+            <v>FT//ex(M3517､M3518､M3519､M3520､M3521)､
+LS550(M3551-A/B/Cﾓﾃﾞﾙ､M3553-Aﾓﾃﾞﾙ､M3554-Aﾓﾃﾞﾙ)､
+XEN-PC(M3456-Cﾓﾃﾞﾙ､M3466-Bﾓﾃﾞﾙ､M3476-Aﾓﾃﾞﾙ)用｡但し､CPUが
+Pentiumの場合は同じ容量のﾒﾓﾘを2個ずつ増設する必要あり｡</v>
           </cell>
           <cell r="F62">
             <v>60000</v>
@@ -17215,7 +17311,10 @@
             <v>16MB増設ﾒﾓﾘｷｯﾄ</v>
           </cell>
           <cell r="E63" t="str">
-            <v>FT//ex(M3516､M3517､M3518､M3519､M3520､M3521)､FT2200､LS550(M3551-A/B/Cﾓﾃﾞﾙ､M3553-Aﾓﾃﾞﾙ､M3554-Aﾓﾃﾞﾙ)､XEN-PC､XEN-LSⅡ用｡16MB(SIMM)×1個｡但し､CPUがPentiumの場合は同じ容量のﾒﾓﾘを2個ずつ増設する必要あり｡</v>
+            <v>FT//ex(M3516､M3517､M3518､M3519､M3520､M3521)､FT2200､
+LS550(M3551-A/B/Cﾓﾃﾞﾙ､M3553-Aﾓﾃﾞﾙ､M3554-Aﾓﾃﾞﾙ)､XEN-PC､
+XEN-LSⅡ用｡16MB(SIMM)×1個｡但し､CPUがPentiumの場合は同じ容量
+のﾒﾓﾘを2個ずつ増設する必要あり｡</v>
           </cell>
           <cell r="F63">
             <v>80000</v>
@@ -17379,7 +17478,10 @@
             <v>32MB増設ﾒﾓﾘｷｯﾄ</v>
           </cell>
           <cell r="E64" t="str">
-            <v>FT//ex(M3517､M3518､M3519､M3520､M3521)､FT2200､LS550(M3551-A/B/Cﾓﾃﾞﾙ､M3553-Aﾓﾃﾞﾙ､M3554-Aﾓﾃﾞﾙ)､XEN-PC(M3456､M3466､M3476)用｡32MB(SIMM)×1個｡但し､CPUがPentiumの場合は同じ容量のﾒﾓﾘを2個ずつ増設する必要あり｡</v>
+            <v>FT//ex(M3517､M3518､M3519､M3520､M3521)､FT2200､
+LS550(M3551-A/B/Cﾓﾃﾞﾙ､M3553-Aﾓﾃﾞﾙ､M3554-Aﾓﾃﾞﾙ)､
+XEN-PC(M3456､M3466､M3476)用｡32MB(SIMM)×1個｡但し､CPUが
+Pentiumの場合は同じ容量のﾒﾓﾘを2個ずつ増設する必要あり｡</v>
           </cell>
           <cell r="F64">
             <v>160000</v>
@@ -18202,7 +18304,8 @@
             <v>8MB増設EDOﾒﾓﾘｷｯﾄ</v>
           </cell>
           <cell r="E69" t="str">
-            <v>AL､EL､SX(M3423-Cﾓﾃﾞﾙ)､FX(M3484-Cﾓﾃﾞﾙ)､GX(M3464-Dﾓﾃﾞﾙ)用。8MB(DIMM)×1個｡</v>
+            <v>AL､EL､SX(M3423-Cﾓﾃﾞﾙ)､FX(M3484-Cﾓﾃﾞﾙ)､GX(M3464-Dﾓﾃﾞﾙ)用。
+8MB(DIMM)×1個｡</v>
           </cell>
           <cell r="F69">
             <v>16000</v>
@@ -18366,7 +18469,8 @@
             <v>16MB増設EDOﾒﾓﾘｷｯﾄ</v>
           </cell>
           <cell r="E70" t="str">
-            <v>AL､EL､SX(M3423-Cﾓﾃﾞﾙ)､FX(M3484-Cﾓﾃﾞﾙ)､GX(M3464-Dﾓﾃﾞﾙ)用。16MB(DIMM)×1個｡</v>
+            <v>AL､EL､SX(M3423-Cﾓﾃﾞﾙ)､FX(M3484-Cﾓﾃﾞﾙ)､GX(M3464-Dﾓﾃﾞﾙ)用。
+16MB(DIMM)×1個｡</v>
           </cell>
           <cell r="F70">
             <v>32000</v>
@@ -18530,7 +18634,8 @@
             <v>32MB増設EDOﾒﾓﾘｷｯﾄ</v>
           </cell>
           <cell r="E71" t="str">
-            <v>AL､EL､SX(M3423-Cﾓﾃﾞﾙ)､FX(M3484-Cﾓﾃﾞﾙ)､GX(M3464-Dﾓﾃﾞﾙ)用。32MB(DIMM)×1個｡</v>
+            <v>AL､EL､SX(M3423-Cﾓﾃﾞﾙ)､FX(M3484-Cﾓﾃﾞﾙ)､GX(M3464-Dﾓﾃﾞﾙ)用。
+32MB(DIMM)×1個｡</v>
           </cell>
           <cell r="F71">
             <v>90000</v>
@@ -18727,7 +18832,8 @@
             <v>AC</v>
           </cell>
           <cell r="P72" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q72">
             <v>0</v>
@@ -18847,7 +18953,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD72" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="73">
@@ -18894,7 +19001,8 @@
             <v>AC</v>
           </cell>
           <cell r="P73" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q73">
             <v>0</v>
@@ -19014,7 +19122,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD73" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="74">
@@ -19228,7 +19337,8 @@
             <v>AC</v>
           </cell>
           <cell r="P75" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q75">
             <v>0</v>
@@ -19348,7 +19458,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD75" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="76">
@@ -19362,7 +19473,8 @@
             <v>8MB増設ﾒﾓﾘｷｯﾄ</v>
           </cell>
           <cell r="E76" t="str">
-            <v>GX(M3464-Bﾓﾃﾞﾙ)､NS(M3452-Bﾓﾃﾞﾙ､M3472-Bﾓﾃﾞﾙ)用｡8MB(DIMM)×1個｡</v>
+            <v>GX(M3464-Bﾓﾃﾞﾙ)､NS(M3452-Bﾓﾃﾞﾙ､M3472-Bﾓﾃﾞﾙ)用｡
+8MB(DIMM)×1個｡</v>
           </cell>
           <cell r="F76">
             <v>60000</v>
@@ -19529,7 +19641,8 @@
             <v>16MB増設ﾒﾓﾘｷｯﾄ</v>
           </cell>
           <cell r="E77" t="str">
-            <v>GX(M3464-Bﾓﾃﾞﾙ)､NS(M3452-Bﾓﾃﾞﾙ､M3472-Bﾓﾃﾞﾙ)用｡16MB(DIMM)×1個｡</v>
+            <v>GX(M3464-Bﾓﾃﾞﾙ)､NS(M3452-Bﾓﾃﾞﾙ､M3472-Bﾓﾃﾞﾙ)用｡
+16MB(DIMM)×1個｡</v>
           </cell>
           <cell r="F77">
             <v>120000</v>
@@ -19696,7 +19809,8 @@
             <v>8MB増設ﾒﾓﾘｷｯﾄ</v>
           </cell>
           <cell r="E78" t="str">
-            <v>SX(M3423-Aﾓﾃﾞﾙ､M3423C)､FX(M3474､M3484-A/Bﾓﾃﾞﾙ)､GX(M3464-Cﾓﾃﾞﾙ)用｡4MB(DIMM)×2個｡</v>
+            <v>SX(M3423-Aﾓﾃﾞﾙ､M3423C)､FX(M3474､M3484-A/Bﾓﾃﾞﾙ)､
+GX(M3464-Cﾓﾃﾞﾙ)用｡4MB(DIMM)×2個｡</v>
           </cell>
           <cell r="F78">
             <v>24000</v>
@@ -19729,7 +19843,8 @@
             <v>AC</v>
           </cell>
           <cell r="P78" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q78">
             <v>0</v>
@@ -19849,7 +19964,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD78" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="79">
@@ -19863,7 +19979,8 @@
             <v>16MB増設ﾒﾓﾘｷｯﾄ</v>
           </cell>
           <cell r="E79" t="str">
-            <v>SX(M3423-Aﾓﾃﾞﾙ､M3423C)､FX(M3474､M3484-A/Bﾓﾃﾞﾙ)､GX(M3464-Cﾓﾃﾞﾙ)用｡8MB(DIMM)×2個｡</v>
+            <v>SX(M3423-Aﾓﾃﾞﾙ､M3423C)､FX(M3474､M3484-A/Bﾓﾃﾞﾙ)､
+GX(M3464-Cﾓﾃﾞﾙ)用｡8MB(DIMM)×2個｡</v>
           </cell>
           <cell r="F79">
             <v>120000</v>
@@ -20030,7 +20147,8 @@
             <v>32MB増設ﾒﾓﾘｷｯﾄ</v>
           </cell>
           <cell r="E80" t="str">
-            <v>SX(M3423-Aﾓﾃﾞﾙ､M3423C)､FX(M3474､M3484-A/Bﾓﾃﾞﾙ)､GX(M3464-B/Cﾓﾃﾞﾙ)用｡16MB(DIMM)×2個｡</v>
+            <v>SX(M3423-Aﾓﾃﾞﾙ､M3423C)､FX(M3474､M3484-A/Bﾓﾃﾞﾙ)､
+GX(M3464-B/Cﾓﾃﾞﾙ)用｡16MB(DIMM)×2個｡</v>
           </cell>
           <cell r="F80">
             <v>240000</v>
@@ -20202,7 +20320,9 @@
             <v>JISｷｰﾎﾞｰﾄﾞ</v>
           </cell>
           <cell r="E82" t="str">
-            <v>FT486-66S/66E､FT//s､FT//e､FT//ex､FT1200､FT2200､FT2400､LS660､LS550､XEN-PC､XEN-LSⅡ､AL､EL、SX､FX､GX､SV用｡JIS配列に準拠｡106ｷｰ｡</v>
+            <v>FT486-66S/66E､FT//s､FT//e､FT//ex､FT1200､FT2200､FT2400､LS660､
+LS550､XEN-PC､XEN-LSⅡ､AL､EL、SX､FX､GX､SV用｡JIS配列に準拠｡
+106ｷｰ｡</v>
           </cell>
           <cell r="F82">
             <v>13000</v>
@@ -20399,7 +20519,8 @@
             <v>AC</v>
           </cell>
           <cell r="P83" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q83">
             <v>0</v>
@@ -20519,7 +20640,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD83" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="84">
@@ -20697,7 +20819,8 @@
             <v>ﾏｳｽ</v>
           </cell>
           <cell r="E85" t="str">
-            <v>FT486-66S/66E､FT//s､FT//e､FT//ex､FT1200､FT2200､FT2400､LS660､LS550､XEN-PC､XEN-LSⅡ､AL､EL､SX､FX､GX､SV､NS用｡PS/2｡</v>
+            <v>FT486-66S/66E､FT//s､FT//e､FT//ex､FT1200､FT2200､FT2400､LS660､
+LS550､XEN-PC､XEN-LSⅡ､AL､EL､SX､FX､GX､SV､NS用｡PS/2｡</v>
           </cell>
           <cell r="F85">
             <v>10000</v>
@@ -20861,7 +20984,10 @@
             <v>IDｶｰﾄﾞﾘｰﾀﾞ</v>
           </cell>
           <cell r="E86" t="str">
-            <v>LS550(M3551､M3553､M3554)､XEN-PC(ﾓﾃﾞﾙにより､制限あり｡)､XEN-LSⅡ(ﾓﾃﾞﾙにより､制限あり｡)､SX(M3423-Aﾓﾃﾞﾙ､M3423C)､FX(M3474､M3484-A/Bﾓﾃﾞﾙ)､GX(M3464-B/Cﾓﾃﾞﾙ)､SV､NS用｡磁気ｶｰﾄﾞ(JIS X6301 X6302 Ⅱ型)の読み取り｡</v>
+            <v>LS550(M3551､M3553､M3554)､XEN-PC(ﾓﾃﾞﾙにより､制限あり｡)､
+XEN-LSⅡ(ﾓﾃﾞﾙにより､制限あり｡)､SX(M3423-Aﾓﾃﾞﾙ､M3423C)､
+FX(M3474､M3484-A/Bﾓﾃﾞﾙ)､GX(M3464-B/Cﾓﾃﾞﾙ)､SV､NS用｡
+磁気ｶｰﾄﾞ(JIS X6301 X6302 Ⅱ型)の読み取り｡</v>
           </cell>
           <cell r="F86">
             <v>98000</v>
@@ -21028,7 +21154,10 @@
             <v>ﾊﾞｰｺｰﾄﾞﾊﾝﾄﾞｽｷｬﾅ</v>
           </cell>
           <cell r="E87" t="str">
-            <v>LS550(M3551､M3553､M3554)､XEN-PC(ﾓﾃﾞﾙにより､制限あり｡)､XEN-LSⅡ(ﾓﾃﾞﾙにより､制限あり｡)､SX(M3423-Aﾓﾃﾞﾙ､M3423C)､FX(M3474､M3484-A/Bﾓﾃﾞﾙ)､GX(M3464-B/Cﾓﾃﾞﾙ)､SV､NS用｡ﾊﾞｰｺｰﾄﾞﾃﾞｰﾀ(NW-7､JAN､CODE39､2OF5)の読み取り｡</v>
+            <v>LS550(M3551､M3553､M3554)､XEN-PC(ﾓﾃﾞﾙにより､制限あり｡)､
+XEN-LSⅡ(ﾓﾃﾞﾙにより､制限あり｡)､SX(M3423-Aﾓﾃﾞﾙ､M3423C)､
+FX(M3474､M3484-A/Bﾓﾃﾞﾙ)､GX(M3464-B/Cﾓﾃﾞﾙ)､SV､NS用｡
+ﾊﾞｰｺｰﾄﾞﾃﾞｰﾀ(NW-7､JAN､CODE39､2OF5)の読み取り｡</v>
           </cell>
           <cell r="F87">
             <v>190000</v>
@@ -21195,7 +21324,10 @@
             <v>ﾊﾝﾄﾞOCR</v>
           </cell>
           <cell r="E88" t="str">
-            <v>LS550(M3551､M3553､M3554)､XEN-PC(ﾓﾃﾞﾙにより､制限あり｡)､XEN-LSⅡ(ﾓﾃﾞﾙにより､制限あり｡)､SX(M3423-Aﾓﾃﾞﾙ､M3423C)､FX(M3474､M3484-A/Bﾓﾃﾞﾙ)､GX(M3464-B/Cﾓﾃﾞﾙ)､SV用｡OCR文字(OCR-Bﾌｫﾝﾄ･ｻｲｽﾞⅠの文字28種類)の読み取り｡</v>
+            <v>LS550(M3551､M3553､M3554)､XEN-PC(ﾓﾃﾞﾙにより､制限あり｡)､
+XEN-LSⅡ(ﾓﾃﾞﾙにより､制限あり｡)､SX(M3423-Aﾓﾃﾞﾙ､M3423C)､
+FX(M3474､M3484-A/Bﾓﾃﾞﾙ)､GX(M3464-B/Cﾓﾃﾞﾙ)､SV用｡
+OCR文字(OCR-Bﾌｫﾝﾄ･ｻｲｽﾞⅠの文字28種類)の読み取り｡</v>
           </cell>
           <cell r="F88">
             <v>580000</v>
@@ -21395,7 +21527,8 @@
             <v>AC</v>
           </cell>
           <cell r="P89" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q89">
             <v>0</v>
@@ -21515,7 +21648,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD89" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="90">
@@ -21562,7 +21696,8 @@
             <v>AC</v>
           </cell>
           <cell r="P90" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q90">
             <v>0</v>
@@ -21682,7 +21817,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD90" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="91">
@@ -21701,7 +21837,8 @@
             <v>15ｲﾝﾁ高解像度ｶﾗｰﾃﾞｨｽﾌﾟﾚｲ</v>
           </cell>
           <cell r="E92" t="str">
-            <v>FT486-66S/66E､FT//s､FT//e､FT//ex､FT1200､FT2200､LS660､LS550､XEN-PC､XEN-LSⅡ､SX､FX､GX､SV､NS用｡</v>
+            <v>FT486-66S/66E､FT//s､FT//e､FT//ex､FT1200､FT2200､LS660､LS550､
+XEN-PC､XEN-LSⅡ､SX､FX､GX､SV､NS用｡</v>
           </cell>
           <cell r="F92">
             <v>60000</v>
@@ -21868,7 +22005,8 @@
             <v>15ｲﾝﾁ高解像度ｶﾗｰﾃﾞｨｽﾌﾟﾚｲ</v>
           </cell>
           <cell r="E93" t="str">
-            <v>FT//ex､FT1200､FT2200､FT2400､LS660､LS550､AL､EL､SX(M3423-Cﾓﾃﾞﾙ､M3423C-A3C0/B181)､FX､GX用｡</v>
+            <v>FT//ex､FT1200､FT2200､FT2400､LS660､LS550､AL､EL､
+SX(M3423-Cﾓﾃﾞﾙ､M3423C-A3C0/B181)､FX､GX用｡</v>
           </cell>
           <cell r="F93">
             <v>56000</v>
@@ -22032,7 +22170,8 @@
             <v>15ｲﾝﾁ高解像度ｶﾗｰﾃﾞｨｽﾌﾟﾚｲ</v>
           </cell>
           <cell r="E94" t="str">
-            <v>FT486-66S/66E､FT//s､FT//e､FT//ex､FT1200､FT2200､LS660､LS550､XEN-PC､XEN-LSⅡ､SX､FX､GX､SV､NS用｡</v>
+            <v>FT486-66S/66E､FT//s､FT//e､FT//ex､FT1200､FT2200､LS660､LS550､
+XEN-PC､XEN-LSⅡ､SX､FX､GX､SV､NS用｡</v>
           </cell>
           <cell r="F94">
             <v>60000</v>
@@ -22199,7 +22338,8 @@
             <v>17ｲﾝﾁ高解像度ｶﾗｰﾃﾞｨｽﾌﾟﾚｲ</v>
           </cell>
           <cell r="E95" t="str">
-            <v>FT1200､FT2200､LS660､LS550､XEN-PC､XEN-LSⅡ(B/C/Dﾓﾃﾞﾙ)､SX､FX､GX､SV､NS用｡</v>
+            <v>FT1200､FT2200､LS660､LS550､XEN-PC､XEN-LSⅡ(B/C/Dﾓﾃﾞﾙ)､SX､
+FX､GX､SV､NS用｡</v>
           </cell>
           <cell r="F95">
             <v>110000</v>
@@ -22366,7 +22506,8 @@
             <v>17ｲﾝﾁ高解像度ｶﾗｰﾃﾞｨｽﾌﾟﾚｲ</v>
           </cell>
           <cell r="E96" t="str">
-            <v>FT1200､FT2200､LS660､LS550､XEN-PC､XEN-LSⅡ､SX､FX､GX､SV､NS用｡</v>
+            <v>FT1200､FT2200､LS660､LS550､XEN-PC､XEN-LSⅡ､SX､FX､GX､SV､
+NS用｡</v>
           </cell>
           <cell r="F96">
             <v>110000</v>
@@ -22533,7 +22674,8 @@
             <v>17ｲﾝﾁ高解像度ｶﾗｰﾃﾞｨｽﾌﾟﾚｲ</v>
           </cell>
           <cell r="E97" t="str">
-            <v>FT//ex､FT1200､FT2200､FT2400､LS660､LS550､AL､EL､SX(M3423-Cﾓﾃﾞﾙ､M3423C-A3C0/B181)､FX､GX用｡ﾀﾞｲﾔﾓﾝﾄﾞﾄﾛﾝ｡</v>
+            <v>FT//ex､FT1200､FT2200､FT2400､LS660､LS550､AL､EL､SX(M3423-Cﾓﾃﾞﾙ､
+M3423C-A3C0/B181)､FX､GX用｡ﾀﾞｲﾔﾓﾝﾄﾞﾄﾛﾝ｡</v>
           </cell>
           <cell r="F97">
             <v>98000</v>
@@ -22697,7 +22839,8 @@
             <v>CRT補助ｹ-ﾌﾞﾙ</v>
           </cell>
           <cell r="E98" t="str">
-            <v>FT486-66S､FT//s､LS660､LS550､XEN-PC､XEN-LSⅡ用｡14ｲﾝﾁCRT､15ｲﾝﾁCRTの電源を本体から供給する場合に使用｡</v>
+            <v>FT486-66S､FT//s､LS660､LS550､XEN-PC､XEN-LSⅡ用｡14ｲﾝﾁCRT､
+15ｲﾝﾁCRTの電源を本体から供給する場合に使用｡</v>
           </cell>
           <cell r="F98">
             <v>5000</v>
@@ -24023,7 +24166,8 @@
             <v>内蔵3.5ｲﾝﾁﾊｰﾄﾞﾃﾞｨｽｸ装置(2GB)</v>
           </cell>
           <cell r="E107" t="str">
-            <v>FT486-66E､FT//e､FT//ex(M3517-A110､M3518-A110､M3519-A120､M3520)､LS550(M3557-Aﾓﾃﾞﾙ)用｡SCSI-2｡</v>
+            <v>FT486-66E､FT//e､FT//ex(M3517-A110､M3518-A110､M3519-A120､
+M3520)､LS550(M3557-Aﾓﾃﾞﾙ)用｡SCSI-2｡</v>
           </cell>
           <cell r="F107">
             <v>180000</v>
@@ -24351,7 +24495,8 @@
             <v>内蔵3.5ｲﾝﾁﾊｰﾄﾞﾃﾞｨｽｸ装置(170MB)</v>
           </cell>
           <cell r="E109" t="str">
-            <v>XEN-LSⅡ用｡但し､XEN-LSⅡ(B/Cﾓﾃﾞﾙ)の場合はHDD増設用BIOS-ROM(B4026)が必要｡</v>
+            <v>XEN-LSⅡ用｡但し､XEN-LSⅡ(B/Cﾓﾃﾞﾙ)の場合はHDD増設用
+BIOS-ROM(B4026)が必要｡</v>
           </cell>
           <cell r="F109">
             <v>70000</v>
@@ -24515,7 +24660,9 @@
             <v>内蔵3.5ｲﾝﾁﾊｰﾄﾞﾃﾞｨｽｸ装置(520MB)</v>
           </cell>
           <cell r="E110" t="str">
-            <v>LS550(M3551-A/B/Cﾓﾃﾞﾙ､M3553-Aﾓﾃﾞﾙ､M3554-Aﾓﾃﾞﾙ)､XEN－PC､XEN-LSⅡ用｡但し､XEN-PC(Aﾓﾃﾞﾙ)､XEN-LSⅡ(B/Cﾓﾃﾞﾙ)の場合はHDD増設用BIOS-ROM(B4026)が必要｡</v>
+            <v>LS550(M3551-A/B/Cﾓﾃﾞﾙ､M3553-Aﾓﾃﾞﾙ､M3554-Aﾓﾃﾞﾙ)､XEN－PC､
+XEN-LSⅡ用｡但し､XEN-PC(Aﾓﾃﾞﾙ)､XEN-LSⅡ(B/Cﾓﾃﾞﾙ)の場合は
+HDD増設用BIOS-ROM(B4026)が必要｡</v>
           </cell>
           <cell r="F110">
             <v>40000</v>
@@ -25669,7 +25816,9 @@
             <v>増設ﾃﾞｨｽｸ･ﾍﾞｲ</v>
           </cell>
           <cell r="E117" t="str">
-            <v>FT2400用｡ﾊｰﾄﾞﾃﾞｨｽｸをﾃﾞｭﾌﾟﾚｯｸｽ構成、または6台以上にする場合に必要｡工場ｵﾌﾟｼｮﾝのため､apricot PCｻｰﾊﾞ H/Wｺﾝﾌｨｸﾞﾚｰｼｮﾝｻｰﾋﾞｽが必要｡</v>
+            <v>FT2400用｡ﾊｰﾄﾞﾃﾞｨｽｸをﾃﾞｭﾌﾟﾚｯｸｽ構成、または6台以上にする場合に
+必要｡工場ｵﾌﾟｼｮﾝのため､apricot PCｻｰﾊﾞ H/Wｺﾝﾌｨｸﾞﾚｰｼｮﾝｻｰﾋﾞｽが
+必要｡</v>
           </cell>
           <cell r="F117">
             <v>78000</v>
@@ -27145,7 +27294,8 @@
             <v>増設高速SCSI制御装置6</v>
           </cell>
           <cell r="E126" t="str">
-            <v>FT//ex(M3517-A110､M3518-A110､M3519-A120､M3520-A120､M3521-A120)､FT2200用｡ Fast Wide SCSI(PCI)｡</v>
+            <v>FT//ex(M3517-A110､M3518-A110､M3519-A120､M3520-A120､
+M3521-A120)､FT2200用｡ Fast Wide SCSI(PCI)｡</v>
           </cell>
           <cell r="F126">
             <v>150000</v>
@@ -27476,7 +27626,8 @@
             <v>増設高速SCSI制御装置</v>
           </cell>
           <cell r="E128" t="str">
-            <v>FT2400用｡ﾊｰﾄﾞﾃﾞｨｽｸをﾃﾞｭﾌﾟﾚｯｸｽ構成、または6台以上にする場合に必要｡Ultra Wide SCSI(PCI)｡</v>
+            <v>FT2400用｡ﾊｰﾄﾞﾃﾞｨｽｸをﾃﾞｭﾌﾟﾚｯｸｽ構成、または6台以上にする場合に
+必要｡Ultra Wide SCSI(PCI)｡</v>
           </cell>
           <cell r="F128">
             <v>150000</v>
@@ -27640,7 +27791,8 @@
             <v>増設高速SCSI制御装置</v>
           </cell>
           <cell r="E129" t="str">
-            <v>FT1200用｡ﾊｰﾄﾞﾃﾞｨｽｸをﾃﾞｭﾌﾟﾚｯｸｽ構成にする場合に必要｡Ultra Wide SCSI(PCI)｡</v>
+            <v>FT1200用｡ﾊｰﾄﾞﾃﾞｨｽｸをﾃﾞｭﾌﾟﾚｯｸｽ構成にする場合に必要｡
+Ultra Wide SCSI(PCI)｡</v>
           </cell>
           <cell r="F129">
             <v>150000</v>
@@ -27804,7 +27956,9 @@
             <v>増設SCSI制御装置</v>
           </cell>
           <cell r="E130" t="str">
-            <v>FT1200､FT2200に内蔵高速ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(M6700-13)､または内臓ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(M6700-15)を増設する場合に必要｡ISA｡但し､FT2200は内臓ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(M6700-15）を未ｻﾎﾟｰﾄ｡</v>
+            <v>FT1200､FT2200に内蔵高速ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(M6700-13)､または
+内臓ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(M6700-15)を増設する場合に必要｡ISA｡
+但し､FT2200は内臓ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(M6700-15）を未ｻﾎﾟｰﾄ｡</v>
           </cell>
           <cell r="F130">
             <v>50000</v>
@@ -27968,7 +28122,8 @@
             <v>増設SCSI制御装置</v>
           </cell>
           <cell r="E131" t="str">
-            <v>FT2400に内蔵ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(M6700-15､またはM6700-16)を増設する場合に必要｡PCI｡</v>
+            <v>FT2400に内蔵ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(M6700-15､またはM6700-16)を増設
+する場合に必要｡PCI｡</v>
           </cell>
           <cell r="F131">
             <v>70000</v>
@@ -28132,7 +28287,8 @@
             <v>増設SCSI制御装置</v>
           </cell>
           <cell r="E132" t="str">
-            <v>LS550(Windows3.1ﾓﾃﾞﾙ)､XEN-PC､XEN-LSⅡに内臓ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(M6700-12)を増設する場合に必要｡ISA｡</v>
+            <v>LS550(Windows3.1ﾓﾃﾞﾙ)､XEN-PC､XEN-LSⅡに内臓ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置
+(M6700-12)を増設する場合に必要｡ISA｡</v>
           </cell>
           <cell r="F132">
             <v>70000</v>
@@ -28165,7 +28321,8 @@
             <v>AC</v>
           </cell>
           <cell r="P132" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q132">
             <v>0</v>
@@ -28285,7 +28442,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD132" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="133">
@@ -28299,7 +28457,8 @@
             <v>増設ﾃﾞｨｽｸｱﾚｲ制御装置</v>
           </cell>
           <cell r="E133" t="str">
-            <v>FT2400用｡工場ｵﾌﾟｼｮﾝのため､apricot PCｻｰﾊﾞ H/Wｺﾝﾌｨｸﾞﾚｰｼｮﾝｻｰﾋﾞｽ(ACS-CONFIG-01)が必要｡</v>
+            <v>FT2400用｡工場ｵﾌﾟｼｮﾝのため､apricot PCｻｰﾊﾞ H/Wｺﾝﾌｨｸﾞﾚｰｼｮﾝｻｰﾋﾞｽ
+(ACS-CONFIG-01)が必要｡</v>
           </cell>
           <cell r="F133">
             <v>360000</v>
@@ -28463,7 +28622,8 @@
             <v>増設ﾃﾞｨｽｸｱﾚｲ制御装置</v>
           </cell>
           <cell r="E134" t="str">
-            <v>FT2200用｡工場ｵﾌﾟｼｮﾝのため､apricot PCｻｰﾊﾞ H/Wｺﾝﾌｨｸﾞﾚｰｼｮﾝｻｰﾋﾞｽ(ACS-CONFIG-01)が必要｡</v>
+            <v>FT2200用｡工場ｵﾌﾟｼｮﾝのため､apricot PCｻｰﾊﾞ H/Wｺﾝﾌｨｸﾞﾚｰｼｮﾝｻｰﾋﾞｽ
+(ACS-CONFIG-01)が必要｡</v>
           </cell>
           <cell r="F134">
             <v>360000</v>
@@ -28624,7 +28784,8 @@
             <v>M6700-15</v>
           </cell>
           <cell r="D135" t="str">
-            <v>内蔵ｽﾄﾘ-ﾐﾝｸﾞﾃ-ﾌﾟ装置(DDS-3)</v>
+            <v>内蔵ｽﾄﾘ-ﾐﾝｸﾞﾃ-ﾌﾟ装置
+(DDS-3)</v>
           </cell>
           <cell r="E135" t="str">
             <v>FT1200､FT2400用｡12GB｡</v>
@@ -28788,7 +28949,8 @@
             <v>M6700-16</v>
           </cell>
           <cell r="D136" t="str">
-            <v>内蔵ｽﾄﾘ-ﾐﾝｸﾞﾃ-ﾌﾟ装置(DDS-3ｵ-ﾄﾛ-ﾀﾞ)</v>
+            <v>内蔵ｽﾄﾘ-ﾐﾝｸﾞﾃ-ﾌﾟ装置
+(DDS-3ｵ-ﾄﾛ-ﾀﾞ)</v>
           </cell>
           <cell r="E136" t="str">
             <v>FT2400用｡DDS-3のDATを最大6台まで搭載可能｡</v>
@@ -28952,10 +29114,12 @@
             <v>M6700-13</v>
           </cell>
           <cell r="D137" t="str">
-            <v>内蔵ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置(DDS-2)</v>
+            <v>内蔵ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置
+(DDS-2)</v>
           </cell>
           <cell r="E137" t="str">
-            <v>FT//ex(M3519､M3520､M3521)､FT1200､FT2200用｡4GB(ﾃﾞｰﾀを圧縮した場合は最大16GB)｡</v>
+            <v>FT//ex(M3519､M3520､M3521)､FT1200､FT2200用｡
+4GB(ﾃﾞｰﾀを圧縮した場合は最大16GB)｡</v>
           </cell>
           <cell r="F137">
             <v>280000</v>
@@ -29119,7 +29283,8 @@
             <v>内蔵高速ｽﾄﾘｰﾐﾝｸﾞﾃｰﾌﾟ装置</v>
           </cell>
           <cell r="E138" t="str">
-            <v>FT486-66S/66E､FT//s､FT//e､FT//ex(M3516､M3517､M3518)用｡2GB(ﾃﾞｰﾀを圧縮した場合は最大8GB)｡</v>
+            <v>FT486-66S/66E､FT//s､FT//e､FT//ex(M3516､M3517､M3518)用｡
+2GB(ﾃﾞｰﾀを圧縮した場合は最大8GB)｡</v>
           </cell>
           <cell r="F138" t="str">
             <v>OPEN価格</v>
@@ -29316,7 +29481,8 @@
             <v>AC</v>
           </cell>
           <cell r="P139" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q139">
             <v>0</v>
@@ -29436,7 +29602,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD139" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="140">
@@ -30273,7 +30440,8 @@
             <v>内蔵CD-ROM装置</v>
           </cell>
           <cell r="E145" t="str">
-            <v>SX(M3423-Aﾓﾃﾞﾙ､M3423C)､FX(M3474､M3484-A/Bﾓﾃﾞﾙ)用｡4倍速(ATAPI)｡</v>
+            <v>SX(M3423-Aﾓﾃﾞﾙ､M3423C)､FX(M3474､M3484-A/Bﾓﾃﾞﾙ)用｡
+4倍速(ATAPI)｡</v>
           </cell>
           <cell r="F145">
             <v>38000</v>
@@ -30306,7 +30474,8 @@
             <v>AC</v>
           </cell>
           <cell r="P145" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q145">
             <v>0</v>
@@ -30426,7 +30595,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD145" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="146">
@@ -30445,7 +30615,9 @@
             <v>ﾌﾟﾛｾｯｻ･ｱｯﾌﾟｸﾞﾚ-ﾄﾞ</v>
           </cell>
           <cell r="E147" t="str">
-            <v>FT1200(M3522-E140/E14N)､FT2400用｡CPU(PentiumPro-200)の内部二次ｷｬｯｼｭ容量を512KBにｱｯﾌﾟｸﾞﾚｰﾄﾞ｡ｱｯﾌﾟｸﾞﾚｰﾄﾞ作業費は25,000円｡</v>
+            <v>FT1200(M3522-E140/E14N)､FT2400用｡CPU(PentiumPro-200)の
+内部二次ｷｬｯｼｭ容量を512KBにｱｯﾌﾟｸﾞﾚｰﾄﾞ｡ｱｯﾌﾟｸﾞﾚｰﾄﾞ作業費は
+25,000円｡</v>
           </cell>
           <cell r="F147">
             <v>398000</v>
@@ -30609,7 +30781,8 @@
             <v>ﾌﾟﾛｾｯｻ･ｱｯﾌﾟｸﾞﾚ-ﾄﾞ</v>
           </cell>
           <cell r="E148" t="str">
-            <v>FT2400用｡2個目のCPU(PentiumPro-200､256KBｷｬｯｼｭ)｡ｱｯﾌﾟｸﾞﾚｰﾄﾞ作業費は25,000円｡</v>
+            <v>FT2400用｡2個目のCPU(PentiumPro-200､256KBｷｬｯｼｭ)｡
+ｱｯﾌﾟｸﾞﾚｰﾄﾞ作業費は25,000円｡</v>
           </cell>
           <cell r="F148">
             <v>198000</v>
@@ -30773,7 +30946,8 @@
             <v>CPU取り付けｷｯﾄ</v>
           </cell>
           <cell r="E149" t="str">
-            <v>FT2400用｡2個目のCPUを増設する場合に必要。CPUﾋｰﾄｼﾝｸ + 電圧変換ﾓｼﾞｭｰﾙ｡</v>
+            <v>FT2400用｡2個目のCPUを増設する場合に必要。
+CPUﾋｰﾄｼﾝｸ + 電圧変換ﾓｼﾞｭｰﾙ｡</v>
           </cell>
           <cell r="F149">
             <v>122000</v>
@@ -30937,7 +31111,9 @@
             <v>ﾌﾟﾛｾｯｻ･ｱｯﾌﾟｸﾞﾚｰﾄﾞ</v>
           </cell>
           <cell r="E150" t="str">
-            <v>FT1200(M3522-A120/A12N)､FT2200用｡CPU(PentiumPro-200)の内部二次ｷｬｯｼｭ容量を512KBにｱｯﾌﾟｸﾞﾚｰﾄﾞ｡ｱｯﾌﾟｸﾞﾚｰﾄﾞ作業費は25,000円｡</v>
+            <v>FT1200(M3522-A120/A12N)､FT2200用｡CPU(PentiumPro-200)の
+内部二次ｷｬｯｼｭ容量を512KBにｱｯﾌﾟｸﾞﾚｰﾄﾞ｡ｱｯﾌﾟｸﾞﾚｰﾄﾞ作業費は
+25,000円｡</v>
           </cell>
           <cell r="F150">
             <v>360000</v>
@@ -31262,7 +31438,8 @@
             <v>B4951-2</v>
           </cell>
           <cell r="D152" t="str">
-            <v>増設ﾃﾞｭｱﾙﾌﾟﾛｾｯｻ(Pentium-150)</v>
+            <v>増設ﾃﾞｭｱﾙﾌﾟﾛｾｯｻ
+(Pentium-150)</v>
           </cell>
           <cell r="E152" t="str">
             <v>FT//ex(M3521)用｡ｱｯﾌﾟｸﾞﾚｰﾄﾞ作業費は25,000円｡</v>
@@ -31426,7 +31603,8 @@
             <v>B4951-1</v>
           </cell>
           <cell r="D153" t="str">
-            <v>増設ﾃﾞｭｱﾙﾌﾟﾛｾｯｻ(Pentium-120)</v>
+            <v>増設ﾃﾞｭｱﾙﾌﾟﾛｾｯｻ
+(Pentium-120)</v>
           </cell>
           <cell r="E153" t="str">
             <v>FT//ex(M3520)用｡ｱｯﾌﾟｸﾞﾚｰﾄﾞ作業費は25,000円｡</v>
@@ -31593,7 +31771,8 @@
             <v>FT486ｼｽﾃﾑROMｱｯﾌﾟｸﾞﾚｰﾄﾞ(WindowsNT対応)</v>
           </cell>
           <cell r="E154" t="str">
-            <v>FT486-66S/66E用｡WindowsNTでHyperRAMｻﾎﾟｰﾄを可能にするためのｼｽﾃﾑROMｱｯﾌﾟｸﾞﾚｰﾄﾞ｡ｱｯﾌﾟｸﾞﾚｰﾄﾞ作業費は28,000円｡</v>
+            <v>FT486-66S/66E用｡WindowsNTでHyperRAMｻﾎﾟｰﾄを可能にするための
+ｼｽﾃﾑROMｱｯﾌﾟｸﾞﾚｰﾄﾞ｡ｱｯﾌﾟｸﾞﾚｰﾄﾞ作業費は28,000円｡</v>
           </cell>
           <cell r="F154">
             <v>8000</v>
@@ -33239,7 +33418,10 @@
             <v>PCI LANﾎﾞｰﾄﾞ</v>
           </cell>
           <cell r="E164" t="str">
-            <v>FT//ex(M3517､M3518､M3519､M3520､M3521)､FT2200､LS550(M3551､M3553､M3554､M3557-Aﾓﾃﾞﾙ)､XEN-PC(M3456､M3466､M3476)用｡10BASE-T/5(PCI)｡但し､LS550､XEN-PCの場合はNetWareｻｰﾊﾞ､WindowsNTｻｰﾊﾞで使用する場合のみ｡</v>
+            <v>FT//ex(M3517､M3518､M3519､M3520､M3521)､FT2200､LS550(M3551､
+M3553､M3554､M3557-Aﾓﾃﾞﾙ)､XEN-PC(M3456､M3466､M3476)用｡
+10BASE-T/5(PCI)｡但し､LS550､XEN-PCの場合はNetWareｻｰﾊﾞ､
+WindowsNTｻｰﾊﾞで使用する場合のみ｡</v>
           </cell>
           <cell r="F164">
             <v>38000</v>
@@ -33406,7 +33588,8 @@
             <v>ISA LANﾎﾞｰﾄﾞ</v>
           </cell>
           <cell r="E165" t="str">
-            <v>LS550(M3551､M3553､M3554､M3557-Aﾓﾃﾞﾙ)､XEN-PC用｡10BASE-T/5(ISA)｡</v>
+            <v>LS550(M3551､M3553､M3554､M3557-Aﾓﾃﾞﾙ)､XEN-PC用｡
+10BASE-T/5(ISA)｡</v>
           </cell>
           <cell r="F165">
             <v>38000</v>
@@ -34226,7 +34409,8 @@
             <v>EISA通信制御装置</v>
           </cell>
           <cell r="E170" t="str">
-            <v>FT//ex(M3516､M3517-A110､M3518-A110､M3519-A120､M3520-A120､M3521-A120)用｡EISA｡</v>
+            <v>FT//ex(M3516､M3517-A110､M3518-A110､M3519-A120､M3520-A120､
+M3521-A120)用｡EISA｡</v>
           </cell>
           <cell r="F170">
             <v>130000</v>
@@ -34390,7 +34574,8 @@
             <v>同期通信ｱﾀﾞﾌﾟﾀ</v>
           </cell>
           <cell r="E171" t="str">
-            <v>FT//ex(M3516)､LS550(M3551､M3553､M3554)､XEN-PC､XEN-LSⅡ用｡ISA｡但し､Windows95は不可｡</v>
+            <v>FT//ex(M3516)､LS550(M3551､M3553､M3554)､XEN-PC､XEN-LSⅡ用｡
+ISA｡但し､Windows95は不可｡</v>
           </cell>
           <cell r="F171">
             <v>60000</v>
@@ -35046,7 +35231,8 @@
             <v>4ﾁｬﾝﾈﾙRS232Cｲﾝﾀﾌｪｰｽ</v>
           </cell>
           <cell r="E175" t="str">
-            <v>LS550(M3551､M3553､M3554､M3557-Aﾓﾃﾞﾙ)､XEN-PC､XEN-LSⅡ用｡ISA｡Windows95は不可｡</v>
+            <v>LS550(M3551､M3553､M3554､M3557-Aﾓﾃﾞﾙ)､XEN-PC､XEN-LSⅡ用｡
+ISA｡Windows95は不可｡</v>
           </cell>
           <cell r="F175">
             <v>80000</v>
@@ -35538,7 +35724,8 @@
             <v>FAX/DATAﾓﾃﾞﾑｶｰﾄﾞ</v>
           </cell>
           <cell r="E178" t="str">
-            <v>AL､EL､SX､FX､GX､SV､NS用｡FAX:14.4Kbps/DATA:28.8Kbps｡PCMCIA TYPEⅡ｡</v>
+            <v>AL､EL､SX､FX､GX､SV､NS用｡FAX:14.4Kbps/DATA:28.8Kbps｡
+PCMCIA TYPEⅡ｡</v>
           </cell>
           <cell r="F178">
             <v>15000</v>
@@ -35571,7 +35758,8 @@
             <v>MI</v>
           </cell>
           <cell r="P178" t="str">
-            <v>保守はｵﾑﾛﾝ対応。</v>
+            <v>保守はｵﾑﾛﾝ
+対応。</v>
           </cell>
           <cell r="Q178">
             <v>0</v>
@@ -35691,7 +35879,8 @@
             <v>MI</v>
           </cell>
           <cell r="BD178" t="str">
-            <v>保守はｵﾑﾛﾝ対応。</v>
+            <v>保守はｵﾑﾛﾝ
+対応。</v>
           </cell>
         </row>
         <row r="179">
@@ -35738,7 +35927,8 @@
             <v>AC</v>
           </cell>
           <cell r="P179" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q179">
             <v>0</v>
@@ -35858,7 +36048,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD179" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="180">
@@ -35905,7 +36096,8 @@
             <v>AC</v>
           </cell>
           <cell r="P180" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q180">
             <v>0</v>
@@ -36025,7 +36217,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD180" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="181">
@@ -36203,7 +36396,8 @@
             <v>ﾓﾃﾞﾑｹｰﾌﾞﾙ</v>
           </cell>
           <cell r="E182" t="str">
-            <v>FT486-66S/66E､FT//s､FT//e､FT//ex､XEN-PC(M3416-Aﾓﾃﾞﾙ､M3426-Aﾓﾃﾞﾙ､M3436-Aﾓﾃﾞﾙ)､XEN-LSⅡ用｡Dｻﾌﾞ25P-25P｡</v>
+            <v>FT486-66S/66E､FT//s､FT//e､FT//ex､XEN-PC(M3416-Aﾓﾃﾞﾙ､
+M3426-Aﾓﾃﾞﾙ､M3436-Aﾓﾃﾞﾙ)､XEN-LSⅡ用｡Dｻﾌﾞ25P-25P｡</v>
           </cell>
           <cell r="F182">
             <v>10000</v>
@@ -36531,7 +36725,9 @@
             <v>ﾓﾃﾞﾑｹｰﾌﾞﾙ</v>
           </cell>
           <cell r="E184" t="str">
-            <v>FT//ex(M3516､M3517)､FT1200､FT2200､FT2400､LS660､LS550､XEN-PC(M3416-Bﾓﾃﾞﾙ､M3436-Bﾓﾃﾞﾙ､M3456､M3466､M3476)､AL､EL､SX､FX､GX､SV､NS用｡Dｻﾌﾞ9P-25P｡RS-232Cｲﾝﾀﾌｪｰｽに接続｡</v>
+            <v>FT//ex(M3516､M3517)､FT1200､FT2200､FT2400､LS660､LS550､
+XEN-PC(M3416-Bﾓﾃﾞﾙ､M3436-Bﾓﾃﾞﾙ､M3456､M3466､M3476)､
+AL､EL､SX､FX､GX､SV､NS用｡Dｻﾌﾞ9P-25P｡RS-232Cｲﾝﾀﾌｪｰｽに接続｡</v>
           </cell>
           <cell r="F184">
             <v>10000</v>
@@ -36695,7 +36891,8 @@
             <v>RS232Cｹｰﾌﾞﾙ</v>
           </cell>
           <cell r="E185" t="str">
-            <v>FT486-66S/66E､FT//s､FT//e､FT//ex､XEN-PC(M3416-Aﾓﾃﾞﾙ､M3426-Aﾓﾃﾞﾙ､M3436-Aﾓﾃﾞﾙ)､XEN-LSⅡ用｡Dｻﾌﾞ25P-25P｡</v>
+            <v>FT486-66S/66E､FT//s､FT//e､FT//ex､XEN-PC(M3416-Aﾓﾃﾞﾙ､
+M3426-Aﾓﾃﾞﾙ､M3436-Aﾓﾃﾞﾙ)､XEN-LSⅡ用｡Dｻﾌﾞ25P-25P｡</v>
           </cell>
           <cell r="F185">
             <v>10000</v>
@@ -36859,7 +37056,9 @@
             <v>RS232Cｹｰﾌﾞﾙ</v>
           </cell>
           <cell r="E186" t="str">
-            <v>FT//ex(M3516､M3517)､FT1200､FT2200､FT2400､LS660､LS550､XEN-PC(M3416-Bﾓﾃﾞﾙ､M3436-Bﾓﾃﾞﾙ､M3456､M3466､M3476)､AL､EL､SX､FX､GX､SV､NS用｡Dｻﾌﾞ9P-25P｡</v>
+            <v>FT//ex(M3516､M3517)､FT1200､FT2200､FT2400､LS660､LS550､
+XEN-PC(M3416-Bﾓﾃﾞﾙ､M3436-Bﾓﾃﾞﾙ､M3456､M3466､M3476)､
+AL､EL､SX､FX､GX､SV､NS用｡Dｻﾌﾞ9P-25P｡</v>
           </cell>
           <cell r="F186">
             <v>10000</v>
@@ -37023,7 +37222,8 @@
             <v>ﾌﾟﾗｸﾞｱﾀﾞﾌﾟﾀ</v>
           </cell>
           <cell r="E187" t="str">
-            <v>FT486-66S/66E､FT//s､FT//e､FT//ex､XEN-PC(M3416-Aﾓﾃﾞﾙ､M3426-Aﾓﾃﾞﾙ､M3436-Aﾓﾃﾞﾙ)､XEN-LSⅡ用｡Dｻﾌﾞ25Pを9Pに変換｡</v>
+            <v>FT486-66S/66E､FT//s､FT//e､FT//ex､XEN-PC(M3416-Aﾓﾃﾞﾙ､
+M3426-Aﾓﾃﾞﾙ､M3436-Aﾓﾃﾞﾙ)､XEN-LSⅡ用｡Dｻﾌﾞ25Pを9Pに変換｡</v>
           </cell>
           <cell r="F187">
             <v>5000</v>
@@ -37356,7 +37556,10 @@
             <v>日本語ﾌﾟﾘﾝﾀ</v>
           </cell>
           <cell r="E190" t="str">
-            <v>FT486-66S/66E､FT//s､FT//e､LS660､LS550､XEN-PC､XEN-LSⅡ用｡24ﾋﾟﾝ･ﾄﾞｯﾄﾏﾄﾘｸｽ漢字ﾌﾟﾘﾝﾀ｡A5縦～B5縦｡漢字45字/秒｡80桁/行｡但し､XEN-PC(M3416-Bﾓﾃﾞﾙ､M3436-Bﾓﾃﾞﾙ)の場合はﾊﾟﾗﾚﾙ入出力ｲﾝﾀﾌｪｰｽ(B8431-1)が必要｡</v>
+            <v>FT486-66S/66E､FT//s､FT//e､LS660､LS550､XEN-PC､XEN-LSⅡ用｡
+24ﾋﾟﾝ･ﾄﾞｯﾄﾏﾄﾘｸｽ漢字ﾌﾟﾘﾝﾀ｡A5縦～B5縦｡漢字45字/秒｡80桁/行｡
+但し､XEN-PC(M3416-Bﾓﾃﾞﾙ､M3436-Bﾓﾃﾞﾙ)の場合はﾊﾟﾗﾚﾙ入出力
+ｲﾝﾀﾌｪｰｽ(B8431-1)が必要｡</v>
           </cell>
           <cell r="F190">
             <v>160000</v>
@@ -37523,7 +37726,10 @@
             <v>日本語ﾌﾟﾘﾝﾀ</v>
           </cell>
           <cell r="E191" t="str">
-            <v>FT486-66S/66E､FT//s､FT//e､LS660､LS550､XEN-PC､XEN-LSⅡ用｡24ﾋﾟﾝ･ﾄﾞｯﾄﾏﾄﾘｸｽ漢字ﾌﾟﾘﾝﾀ｡A5縦～B4横｡漢字45字/秒｡136桁/行｡但し､XEN-PC(M3416-Bﾓﾃﾞﾙ､M3436-Bﾓﾃﾞﾙ)の場合はﾊﾟﾗﾚﾙ入出力ｲﾝﾀﾌｪｰｽ(B8431-1)が必要｡</v>
+            <v>FT486-66S/66E､FT//s､FT//e､LS660､LS550､XEN-PC､XEN-LSⅡ用｡
+24ﾋﾟﾝ･ﾄﾞｯﾄﾏﾄﾘｸｽ漢字ﾌﾟﾘﾝﾀ｡A5縦～B4横｡漢字45字/秒｡136桁/行｡
+但し､XEN-PC(M3416-Bﾓﾃﾞﾙ､M3436-Bﾓﾃﾞﾙ)の場合はﾊﾟﾗﾚﾙ入出力
+ｲﾝﾀﾌｪｰｽ(B8431-1)が必要｡</v>
           </cell>
           <cell r="F191">
             <v>180000</v>
@@ -37687,7 +37893,10 @@
             <v>日本語ﾌﾟﾘﾝﾀ</v>
           </cell>
           <cell r="E192" t="str">
-            <v>FT486-66S/66E､FT//s､FT//e､LS660､LS550､XEN-PC､XEN-LSⅡ用｡24ﾋﾟﾝ･ﾄﾞｯﾄﾏﾄﾘｸｽ漢字ﾌﾟﾘﾝﾀ｡A5縦～B4横｡漢字100字/秒｡136桁/行｡但し､XEN-PC(M3416-Bﾓﾃﾞﾙ､M3436-Bﾓﾃﾞﾙ)の場合はﾊﾟﾗﾚﾙ入出力ｲﾝﾀﾌｪｰｽ(B8431-1)が必要｡</v>
+            <v>FT486-66S/66E､FT//s､FT//e､LS660､LS550､XEN-PC､XEN-LSⅡ用｡
+24ﾋﾟﾝ･ﾄﾞｯﾄﾏﾄﾘｸｽ漢字ﾌﾟﾘﾝﾀ｡A5縦～B4横｡漢字100字/秒｡136桁/行｡
+但し､XEN-PC(M3416-Bﾓﾃﾞﾙ､M3436-Bﾓﾃﾞﾙ)の場合はﾊﾟﾗﾚﾙ入出力
+ｲﾝﾀﾌｪｰｽ(B8431-1)が必要｡</v>
           </cell>
           <cell r="F192">
             <v>670000</v>
@@ -37851,7 +38060,10 @@
             <v>OA日本語ﾌﾟﾘﾝﾀ</v>
           </cell>
           <cell r="E193" t="str">
-            <v>FT486-66S/66E､FT//s､FT//e､LS550(M3551､M3553､M3554)､XEN-PC､XEN-LSⅡ用｡24ﾋﾟﾝ･ﾄﾞｯﾄﾏﾄﾘｸｽ漢字ﾌﾟﾘﾝﾀ｡A5縦～B4横｡漢字120字/秒｡136桁/行｡水平ｲﾝｻｰﾀ方式｡但し､XEN-PC(M3416-Bﾓﾃﾞﾙ､M3436-Bﾓﾃﾞﾙ)の場合はﾊﾟﾗﾚﾙ入出力ｲﾝﾀﾌｪｰｽ(B8431-1)が必要｡</v>
+            <v>FT486-66S/66E､FT//s､FT//e､LS550(M3551､M3553､M3554)､XEN-PC､
+XEN-LSⅡ用｡24ﾋﾟﾝ･ﾄﾞｯﾄﾏﾄﾘｸｽ漢字ﾌﾟﾘﾝﾀ｡A5縦～B4横｡漢字120字/秒｡
+136桁/行｡水平ｲﾝｻｰﾀ方式｡但し､XEN-PC(M3416-Bﾓﾃﾞﾙ､M3436-Bﾓﾃﾞﾙ)
+の場合はﾊﾟﾗﾚﾙ入出力ｲﾝﾀﾌｪｰｽ(B8431-1)が必要｡</v>
           </cell>
           <cell r="F193">
             <v>1150000</v>
@@ -38018,7 +38230,8 @@
             <v>日本語ﾗｲﾝﾌﾟﾘﾝﾀ</v>
           </cell>
           <cell r="E194" t="str">
-            <v>FT//s､FT//e､FT//ex（M3517､M3518､M3519､M3520､M3521)､LS660､LS550､XEN-PC､XEN-LSⅡ用｡430行/分(高速ﾓｰﾄﾞ)｡</v>
+            <v>FT//s､FT//e､FT//ex（M3517､M3518､M3519､M3520､M3521)､LS660､
+LS550､XEN-PC､XEN-LSⅡ用｡430行/分(高速ﾓｰﾄﾞ)｡</v>
           </cell>
           <cell r="F194">
             <v>2998000</v>
@@ -38182,7 +38395,8 @@
             <v>ﾌﾟﾘﾝﾀｹｰﾌﾞﾙ</v>
           </cell>
           <cell r="E195" t="str">
-            <v>日本語ﾌﾟﾘﾝﾀ(M6261-1､M6265-1､M6267-1)､OA日本語ﾌﾟﾘﾝﾀ(M6268-1)､ﾍﾟｰｼﾞﾌﾟﾘﾝﾀ(M6257-1)､日本語ﾗｲﾝﾌﾟﾘﾝﾀ(M6611-1)用｡3m｡</v>
+            <v>日本語ﾌﾟﾘﾝﾀ(M6261-1､M6265-1､M6267-1)､OA日本語ﾌﾟﾘﾝﾀ(M6268-1)､
+ﾍﾟｰｼﾞﾌﾟﾘﾝﾀ(M6257-1)､日本語ﾗｲﾝﾌﾟﾘﾝﾀ(M6611-1)用｡3m｡</v>
           </cell>
           <cell r="F195">
             <v>10000</v>
@@ -38843,7 +39057,8 @@
             <v>増設電源装置</v>
           </cell>
           <cell r="E200" t="str">
-            <v>FT2400用｡ﾊｰﾄﾞﾃﾞｨｽｸを6台以上､または電源を冗長構成にする場合に必要｡</v>
+            <v>FT2400用｡ﾊｰﾄﾞﾃﾞｨｽｸを6台以上､または電源を冗長構成にする場合
+に必要｡</v>
           </cell>
           <cell r="F200">
             <v>50000</v>
@@ -39007,7 +39222,8 @@
             <v>増設ﾌｧﾝｷｯﾄ</v>
           </cell>
           <cell r="E201" t="str">
-            <v>FT2400用｡電源を増設する場合に使用するﾌｧﾝ(×2個)とその取り付けｷｯﾄ｡</v>
+            <v>FT2400用｡電源を増設する場合に使用するﾌｧﾝ(×2個)と
+その取り付けｷｯﾄ｡</v>
           </cell>
           <cell r="F201">
             <v>20000</v>
@@ -39171,7 +39387,9 @@
             <v>電源増設ｷｯﾄ</v>
           </cell>
           <cell r="E202" t="str">
-            <v>FT2400用｡2個目の電源を増設する場合に必要｡(3個目の電源を増設する場合は不要。)増設ﾌｧﾝｷｯﾄ(RFAN-29)付き｡工場ｵﾌﾟｼｮﾝのため､apricot PCｻｰﾊﾞ H/Wｺﾝﾌｨｸﾞﾚｰｼｮﾝｻｰﾋﾞｽが必要｡</v>
+            <v>FT2400用｡2個目の電源を増設する場合に必要｡
+(3個目の電源を増設する場合は不要。)増設ﾌｧﾝｷｯﾄ(RFAN-29)付き｡
+工場ｵﾌﾟｼｮﾝのため､apricot PCｻｰﾊﾞ H/Wｺﾝﾌｨｸﾞﾚｰｼｮﾝｻｰﾋﾞｽが必要｡</v>
           </cell>
           <cell r="F202">
             <v>100000</v>
@@ -40024,7 +40242,8 @@
             <v>AC</v>
           </cell>
           <cell r="P207" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q207">
             <v>0</v>
@@ -40144,7 +40363,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD207" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="208">
@@ -40191,7 +40411,8 @@
             <v>AC</v>
           </cell>
           <cell r="P208" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q208">
             <v>0</v>
@@ -40311,7 +40532,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD208" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="209">
@@ -40358,7 +40580,8 @@
             <v>AC</v>
           </cell>
           <cell r="P209" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q209">
             <v>0</v>
@@ -40478,7 +40701,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD209" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="210">
@@ -40525,7 +40749,8 @@
             <v>AC</v>
           </cell>
           <cell r="P210" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q210">
             <v>0</v>
@@ -40645,7 +40870,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD210" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="211">
@@ -40659,7 +40885,8 @@
             <v>内蔵ﾊﾞｯﾃﾘ</v>
           </cell>
           <cell r="E211" t="str">
-            <v>SX(M3423-Aﾓﾃﾞﾙ､M3423C)､FX(M3474､M3484-A/Bﾓﾃﾞﾙ)用｡Ni-MHﾊﾞｯﾃﾘ｡</v>
+            <v>SX(M3423-Aﾓﾃﾞﾙ､M3423C)､FX(M3474､M3484-A/Bﾓﾃﾞﾙ)用｡
+Ni-MHﾊﾞｯﾃﾘ｡</v>
           </cell>
           <cell r="F211">
             <v>15000</v>
@@ -40692,7 +40919,8 @@
             <v>AC</v>
           </cell>
           <cell r="P211" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q211">
             <v>0</v>
@@ -40812,7 +41040,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD211" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="212">
@@ -41515,7 +41744,8 @@
             <v>AC</v>
           </cell>
           <cell r="P216" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q216">
             <v>0</v>
@@ -41635,7 +41865,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD216" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="217">
@@ -41682,7 +41913,8 @@
             <v>AC</v>
           </cell>
           <cell r="P217" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
           <cell r="Q217">
             <v>0</v>
@@ -41802,7 +42034,8 @@
             <v>AC</v>
           </cell>
           <cell r="BD217" t="str">
-            <v>在庫終了次第、販売終了</v>
+            <v>在庫終了次第、
+販売終了</v>
           </cell>
         </row>
         <row r="218">
@@ -42638,10 +42871,12 @@
             <v>････</v>
           </cell>
           <cell r="D224" t="str">
-            <v>FT2400 ﾓﾃﾞﾙ6200-40Nﾛｰﾀｽﾉｰﾂｾｯﾄﾓﾃﾞﾙ</v>
+            <v>FT2400 ﾓﾃﾞﾙ6200-40N
+ﾛｰﾀｽﾉｰﾂｾｯﾄﾓﾃﾞﾙ</v>
           </cell>
           <cell r="E224" t="str">
-            <v>FT2400 ﾓﾃﾞﾙ 6200-40N(M3529-A14N)､ﾛｰﾀｽﾉｰﾂ R4.5(ｲﾝｽﾄｰﾙｷｯﾄ､ｼﾝｸﾞﾙﾌﾟﾛｾｯｻ版のｻｰﾊﾞ1ﾗｲｾﾝｽ､ｸﾗｲｱﾝﾄ1ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
+            <v>FT2400 ﾓﾃﾞﾙ 6200-40N(M3529-A14N)､ﾛｰﾀｽﾉｰﾂ R4.5
+(ｲﾝｽﾄｰﾙｷｯﾄ､ｼﾝｸﾞﾙﾌﾟﾛｾｯｻ版のｻｰﾊﾞ1ﾗｲｾﾝｽ､ｸﾗｲｱﾝﾄ1ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
           </cell>
           <cell r="F224">
             <v>1516000</v>
@@ -42802,10 +43037,12 @@
             <v>････</v>
           </cell>
           <cell r="D225" t="str">
-            <v>FT2400 ﾓﾃﾞﾙ6200-40NMS Exchangeｾｯﾄﾓﾃﾞﾙ</v>
+            <v>FT2400 ﾓﾃﾞﾙ6200-40N
+MS Exchangeｾｯﾄﾓﾃﾞﾙ</v>
           </cell>
           <cell r="E225" t="str">
-            <v>FT2400 ﾓﾃﾞﾙ 6200-40N(M3529-A14N)､MS Exchange Server 4.0ｲﾝﾄﾛﾊﾟｯｸ（ｻｰﾊﾞ1ﾗｲｾﾝｽ､ｸﾗｲｱﾝﾄ5ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
+            <v>FT2400 ﾓﾃﾞﾙ 6200-40N(M3529-A14N)､MS Exchange Server 4.0
+ｲﾝﾄﾛﾊﾟｯｸ（ｻｰﾊﾞ1ﾗｲｾﾝｽ､ｸﾗｲｱﾝﾄ5ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
           </cell>
           <cell r="F225">
             <v>1487000</v>
@@ -42966,10 +43203,13 @@
             <v>････</v>
           </cell>
           <cell r="D226" t="str">
-            <v>FT2200 ﾓﾃﾞﾙ6200-20Nﾛｰﾀｽﾉｰﾂｾｯﾄﾓﾃﾞﾙ</v>
+            <v>FT2200 ﾓﾃﾞﾙ6200-20N
+ﾛｰﾀｽﾉｰﾂｾｯﾄﾓﾃﾞﾙ</v>
           </cell>
           <cell r="E226" t="str">
-            <v>FT2200 ﾓﾃﾞﾙ 6200-20N(M3528-A12N)､ﾌｧｽﾄｲｰｻﾈｯﾄ･ｱﾀﾞﾌﾟﾀ(AC-905-TX2)､ﾛｰﾀｽﾉｰﾂ R4.5(ｲﾝｽﾄｰﾙｷｯﾄ､ｼﾝｸﾞﾙﾌﾟﾛｾｯｻ版のｻｰﾊﾞ1ﾗｲｾﾝｽ､ｸﾗｲｱﾝﾄ1ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
+            <v>FT2200 ﾓﾃﾞﾙ 6200-20N(M3528-A12N)､ﾌｧｽﾄｲｰｻﾈｯﾄ･ｱﾀﾞﾌﾟﾀ
+(AC-905-TX2)､ﾛｰﾀｽﾉｰﾂ R4.5(ｲﾝｽﾄｰﾙｷｯﾄ､ｼﾝｸﾞﾙﾌﾟﾛｾｯｻ版の
+ｻｰﾊﾞ1ﾗｲｾﾝｽ､ｸﾗｲｱﾝﾄ1ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
           </cell>
           <cell r="F226">
             <v>1596000</v>
@@ -43130,10 +43370,13 @@
             <v>････</v>
           </cell>
           <cell r="D227" t="str">
-            <v>FT2200 ﾓﾃﾞﾙ6200-20NMS Exchangeｾｯﾄﾓﾃﾞﾙ</v>
+            <v>FT2200 ﾓﾃﾞﾙ6200-20N
+MS Exchangeｾｯﾄﾓﾃﾞﾙ</v>
           </cell>
           <cell r="E227" t="str">
-            <v>FT2200 ﾓﾃﾞﾙ 6200-20N(M3528-A12N)､ﾌｧｽﾄｲｰｻﾈｯﾄ･ｱﾀﾞﾌﾟﾀ(AC-905-TX2)､MS Exchange Server 4.0ｲﾝﾄﾛﾊﾟｯｸ（ｻｰﾊﾞ1ﾗｲｾﾝｽ､ｸﾗｲｱﾝﾄ5ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
+            <v>FT2200 ﾓﾃﾞﾙ 6200-20N(M3528-A12N)､ﾌｧｽﾄｲｰｻﾈｯﾄ･ｱﾀﾞﾌﾟﾀ
+(AC-905-TX2)､MS Exchange Server 4.0ｲﾝﾄﾛﾊﾟｯｸ（ｻｰﾊﾞ1ﾗｲｾﾝｽ､
+ｸﾗｲｱﾝﾄ5ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
           </cell>
           <cell r="F227">
             <v>1567000</v>
@@ -43294,10 +43537,12 @@
             <v>････</v>
           </cell>
           <cell r="D228" t="str">
-            <v>FT1200 ﾓﾃﾞﾙ6200-40Nﾛｰﾀｽﾉｰﾂｾｯﾄﾓﾃﾞﾙ</v>
+            <v>FT1200 ﾓﾃﾞﾙ6200-40N
+ﾛｰﾀｽﾉｰﾂｾｯﾄﾓﾃﾞﾙ</v>
           </cell>
           <cell r="E228" t="str">
-            <v>FT1200 ﾓﾃﾞﾙ 6200-40N(M3522-E14N)､ﾛｰﾀｽﾉｰﾂ R4.5(ｲﾝｽﾄｰﾙｷｯﾄ､ｼﾝｸﾞﾙﾌﾟﾛｾｯｻ版のｻｰﾊﾞ1ﾗｲｾﾝｽ､ｸﾗｲｱﾝﾄ1ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
+            <v>FT1200 ﾓﾃﾞﾙ 6200-40N(M3522-E14N)､ﾛｰﾀｽﾉｰﾂ R4.5
+(ｲﾝｽﾄｰﾙｷｯﾄ､ｼﾝｸﾞﾙﾌﾟﾛｾｯｻ版のｻｰﾊﾞ1ﾗｲｾﾝｽ､ｸﾗｲｱﾝﾄ1ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
           </cell>
           <cell r="F228">
             <v>956000</v>
@@ -43458,10 +43703,12 @@
             <v>････</v>
           </cell>
           <cell r="D229" t="str">
-            <v>FT1200 ﾓﾃﾞﾙ6200-40NMS Exchangeｾｯﾄﾓﾃﾞﾙ</v>
+            <v>FT1200 ﾓﾃﾞﾙ6200-40N
+MS Exchangeｾｯﾄﾓﾃﾞﾙ</v>
           </cell>
           <cell r="E229" t="str">
-            <v>FT1200 ﾓﾃﾞﾙ 6200-40N(M3522-E14N)､MS Exchange Server 4.0ｲﾝﾄﾛﾊﾟｯｸ（ｻｰﾊﾞ1ﾗｲｾﾝｽ､ｸﾗｲｱﾝﾄ5ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
+            <v>FT1200 ﾓﾃﾞﾙ 6200-40N(M3522-E14N)､MS Exchange Server 4.0
+ｲﾝﾄﾛﾊﾟｯｸ（ｻｰﾊﾞ1ﾗｲｾﾝｽ､ｸﾗｲｱﾝﾄ5ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
           </cell>
           <cell r="F229">
             <v>927000</v>
@@ -43622,10 +43869,13 @@
             <v>････</v>
           </cell>
           <cell r="D230" t="str">
-            <v>FT1200 ﾓﾃﾞﾙ6200-20Nﾛｰﾀｽﾉｰﾂｾｯﾄﾓﾃﾞﾙ</v>
+            <v>FT1200 ﾓﾃﾞﾙ6200-20N
+ﾛｰﾀｽﾉｰﾂｾｯﾄﾓﾃﾞﾙ</v>
           </cell>
           <cell r="E230" t="str">
-            <v>FT1200 ﾓﾃﾞﾙ 6200-20N(M3522-A12N)､ﾌｧｽﾄｲｰｻﾈｯﾄ･ｱﾀﾞﾌﾟﾀ(AC-905-TX2)､ﾛｰﾀｽﾉｰﾂ R4.5(ｲﾝｽﾄｰﾙｷｯﾄ､ｼﾝｸﾞﾙﾌﾟﾛｾｯｻ版のｻｰﾊﾞ1ﾗｲｾﾝｽ､ｸﾗｲｱﾝﾄ1ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
+            <v>FT1200 ﾓﾃﾞﾙ 6200-20N(M3522-A12N)､ﾌｧｽﾄｲｰｻﾈｯﾄ･ｱﾀﾞﾌﾟﾀ
+(AC-905-TX2)､ﾛｰﾀｽﾉｰﾂ R4.5(ｲﾝｽﾄｰﾙｷｯﾄ､ｼﾝｸﾞﾙﾌﾟﾛｾｯｻ版の
+ｻｰﾊﾞ1ﾗｲｾﾝｽ､ｸﾗｲｱﾝﾄ1ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
           </cell>
           <cell r="F230">
             <v>956000</v>
@@ -43789,10 +44039,13 @@
             <v>････</v>
           </cell>
           <cell r="D231" t="str">
-            <v>FT1200 ﾓﾃﾞﾙ6200-20NMS Exchangeｾｯﾄﾓﾃﾞﾙ</v>
+            <v>FT1200 ﾓﾃﾞﾙ6200-20N
+MS Exchangeｾｯﾄﾓﾃﾞﾙ</v>
           </cell>
           <cell r="E231" t="str">
-            <v>FT1200 ﾓﾃﾞﾙ 6200-20N(M3522-A12N)､ﾌｧｽﾄｲｰｻﾈｯﾄ･ｱﾀﾞﾌﾟﾀ(AC-905-TX2)､MS Exchange Server 4.0 ｲﾝﾄﾛﾊﾟｯｸ（ｻｰﾊﾞ1ﾗｲｾﾝｽ､ｸﾗｲｱﾝﾄ5ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
+            <v>FT1200 ﾓﾃﾞﾙ 6200-20N(M3522-A12N)､ﾌｧｽﾄｲｰｻﾈｯﾄ･ｱﾀﾞﾌﾟﾀ
+(AC-905-TX2)､MS Exchange Server 4.0 ｲﾝﾄﾛﾊﾟｯｸ（ｻｰﾊﾞ1ﾗｲｾﾝｽ､
+ｸﾗｲｱﾝﾄ5ﾗｲｾﾝｽ)ﾊﾞﾝﾄﾞﾙ</v>
           </cell>
           <cell r="F231">
             <v>927000</v>
@@ -44310,9 +44563,7 @@
   </sheetPr>
   <dimension ref="C2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12"/>
   <cols>

</xml_diff>